<commit_message>
small improvement to consulting page
</commit_message>
<xml_diff>
--- a/_site/compounding_growth_10_percent.xlsx
+++ b/_site/compounding_growth_10_percent.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zablotski/Library/Mobile Documents/com~apple~CloudDocs/7. Hobby/programming and stats/yuzaR-Blog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48919B97-091A-4E47-9DE9-5051C74F6523}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCAD22BD-2FB4-AF43-B4CE-9F2B071A3DB3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{EDD741CF-9DB9-2945-BF15-255A1807DC69}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="109">
   <si>
     <t>year</t>
   </si>
@@ -88,9 +88,6 @@
     <t>difference</t>
   </si>
   <si>
-    <t>Consulting</t>
-  </si>
-  <si>
     <t>adds</t>
   </si>
   <si>
@@ -335,6 +332,27 @@
   </si>
   <si>
     <t>$58.58</t>
+  </si>
+  <si>
+    <t>yearly_earnings</t>
+  </si>
+  <si>
+    <t>years_adds</t>
+  </si>
+  <si>
+    <t>years_super_thanks</t>
+  </si>
+  <si>
+    <t>years_koji</t>
+  </si>
+  <si>
+    <t>consulting</t>
+  </si>
+  <si>
+    <t>years_consulting</t>
+  </si>
+  <si>
+    <t>years_total</t>
   </si>
 </sst>
 </file>
@@ -717,10 +735,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6A4B67E-A70E-FF47-86DD-9BF22E85C9FF}">
-  <dimension ref="A1:J97"/>
+  <dimension ref="A1:P97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="178" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -734,9 +752,14 @@
     <col min="7" max="7" width="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.1640625" customWidth="1"/>
     <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -750,7 +773,7 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F1" t="s">
         <v>16</v>
@@ -759,7 +782,7 @@
         <v>17</v>
       </c>
       <c r="H1" t="s">
-        <v>20</v>
+        <v>106</v>
       </c>
       <c r="I1" t="s">
         <v>18</v>
@@ -767,8 +790,26 @@
       <c r="J1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" t="s">
+        <v>102</v>
+      </c>
+      <c r="L1" t="s">
+        <v>103</v>
+      </c>
+      <c r="M1" t="s">
+        <v>104</v>
+      </c>
+      <c r="N1" t="s">
+        <v>105</v>
+      </c>
+      <c r="O1" t="s">
+        <v>107</v>
+      </c>
+      <c r="P1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
       <c r="A2">
         <v>1</v>
       </c>
@@ -801,8 +842,31 @@
         <f>I2-D2</f>
         <v>-1.3499999999999996</v>
       </c>
-    </row>
-    <row r="3" spans="1:10">
+      <c r="K2">
+        <v>2023</v>
+      </c>
+      <c r="L2">
+        <f>SUM(E2:E13)</f>
+        <v>187.62</v>
+      </c>
+      <c r="M2">
+        <f>SUM(F2:F13)</f>
+        <v>4.93</v>
+      </c>
+      <c r="N2">
+        <f>SUM(G2:G13)</f>
+        <v>38</v>
+      </c>
+      <c r="O2">
+        <f>SUM(H2:H13)</f>
+        <v>250</v>
+      </c>
+      <c r="P2">
+        <f>SUM(I2:I13)</f>
+        <v>480.55000000000007</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
       <c r="A3">
         <v>2</v>
       </c>
@@ -836,8 +900,11 @@
         <f t="shared" ref="J3:J4" si="1">I3-D3</f>
         <v>12.350000000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="K3">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
       <c r="A4">
         <v>3</v>
       </c>
@@ -872,7 +939,7 @@
         <v>5.3699999999999974</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:16">
       <c r="A5">
         <v>4</v>
       </c>
@@ -907,7 +974,7 @@
         <v>23.724999999999994</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:16">
       <c r="A6">
         <v>5</v>
       </c>
@@ -942,7 +1009,7 @@
         <v>3.9184999999999945</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:16">
       <c r="A7">
         <v>6</v>
       </c>
@@ -977,7 +1044,7 @@
         <v>258.11234999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:16">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1012,7 +1079,7 @@
         <v>8.6465849999999875</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:16">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1047,7 +1114,7 @@
         <v>-1.7607565000000172</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:16">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1073,7 +1140,7 @@
         <v>-32.153832150000021</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:16">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1099,7 +1166,7 @@
         <v>-35.369215365000024</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:16">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1125,7 +1192,7 @@
         <v>-38.906136901500027</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:16">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1151,7 +1218,7 @@
         <v>-42.796750591650031</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:16">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1166,7 +1233,7 @@
         <v>47.07642565081504</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:16">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1181,7 +1248,7 @@
         <v>51.784068215896546</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:16">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2435,461 +2502,461 @@
   <sheetData>
     <row r="1" spans="1:5" ht="17">
       <c r="A1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18">
       <c r="A2" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="4">
         <v>823</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="18">
       <c r="A3" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="4">
         <v>301</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="17">
       <c r="A4" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B4" s="5">
         <v>246</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>37</v>
-      </c>
       <c r="E4" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="17">
       <c r="A5" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" s="5">
         <v>246</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>37</v>
-      </c>
       <c r="E5" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="17">
       <c r="A6" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" s="5">
         <v>135</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>41</v>
-      </c>
       <c r="E6" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="18">
       <c r="A7" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" s="4">
         <v>110</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>44</v>
-      </c>
       <c r="E7" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="17">
       <c r="A8" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8" s="5">
         <v>110</v>
       </c>
       <c r="C8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>47</v>
-      </c>
       <c r="E8" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="17">
       <c r="A9" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9" s="5">
         <v>110</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>47</v>
-      </c>
       <c r="E9" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="17">
       <c r="A10" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B10" s="5">
         <v>110</v>
       </c>
       <c r="C10" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>51</v>
-      </c>
       <c r="E10" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="17">
       <c r="A11" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B11" s="5">
         <v>90.5</v>
       </c>
       <c r="C11" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>54</v>
-      </c>
       <c r="E11" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="17">
       <c r="A12" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B12" s="5">
         <v>74</v>
       </c>
       <c r="C12" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>57</v>
-      </c>
       <c r="E12" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="17">
       <c r="A13" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B13" s="5">
         <v>60.5</v>
       </c>
       <c r="C13" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="E13" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="17">
       <c r="A14" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B14" s="5">
         <v>60.5</v>
       </c>
       <c r="C14" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>63</v>
-      </c>
       <c r="E14" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="17">
       <c r="A15" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B15" s="5">
         <v>49.5</v>
       </c>
       <c r="C15" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>66</v>
-      </c>
       <c r="E15" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="17">
       <c r="A16" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B16" s="5">
         <v>33.1</v>
       </c>
       <c r="C16" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>69</v>
-      </c>
       <c r="E16" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="17">
       <c r="A17" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B17" s="5">
         <v>33.1</v>
       </c>
       <c r="C17" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>72</v>
-      </c>
       <c r="E17" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="17">
       <c r="A18" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B18" s="5">
         <v>27.1</v>
       </c>
       <c r="C18" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>75</v>
-      </c>
       <c r="E18" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="17">
       <c r="A19" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B19" s="5">
         <v>27.1</v>
       </c>
       <c r="C19" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="D19" s="5" t="s">
-        <v>78</v>
-      </c>
       <c r="E19" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="17">
       <c r="A20" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B20" s="5">
         <v>27.1</v>
       </c>
       <c r="C20" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>81</v>
-      </c>
       <c r="E20" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="17">
       <c r="A21" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B21" s="5">
         <v>9.9</v>
       </c>
       <c r="C21" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="D21" s="5" t="s">
-        <v>84</v>
-      </c>
       <c r="E21" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="17">
       <c r="A22" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B22" s="5">
         <v>6.6</v>
       </c>
       <c r="C22" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>87</v>
-      </c>
       <c r="E22" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="17">
       <c r="A23" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B23" s="5">
         <v>6.6</v>
       </c>
       <c r="C23" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="D23" s="5" t="s">
-        <v>90</v>
-      </c>
       <c r="E23" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="17">
       <c r="A24" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B24" s="5">
         <v>5.4</v>
       </c>
       <c r="C24" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D24" s="5" t="s">
-        <v>93</v>
-      </c>
       <c r="E24" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="17">
       <c r="A25" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B25" s="5">
         <v>5.4</v>
       </c>
       <c r="C25" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D25" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="D25" s="5" t="s">
-        <v>96</v>
-      </c>
       <c r="E25" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="17">
       <c r="A26" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B26" s="5">
         <v>4.4000000000000004</v>
       </c>
       <c r="C26" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D26" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>99</v>
-      </c>
       <c r="E26" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="17">
       <c r="A27" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B27" s="5">
         <v>4.4000000000000004</v>
       </c>
       <c r="C27" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D27" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="D27" s="5" t="s">
-        <v>102</v>
-      </c>
       <c r="E27" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
slow rstudio after long not opening the project
</commit_message>
<xml_diff>
--- a/_site/compounding_growth_10_percent.xlsx
+++ b/_site/compounding_growth_10_percent.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zablotski/Library/Mobile Documents/com~apple~CloudDocs/7. Hobby/programming and stats/yuzaR-Blog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCAD22BD-2FB4-AF43-B4CE-9F2B071A3DB3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C4EA502-2A17-F444-88A0-0AC49DE02AD0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{EDD741CF-9DB9-2945-BF15-255A1807DC69}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="111">
   <si>
     <t>year</t>
   </si>
@@ -73,9 +73,6 @@
     <t>Dez</t>
   </si>
   <si>
-    <t>row_number</t>
-  </si>
-  <si>
     <t>super_thanks</t>
   </si>
   <si>
@@ -353,6 +350,15 @@
   </si>
   <si>
     <t>years_total</t>
+  </si>
+  <si>
+    <t>sponsorship</t>
+  </si>
+  <si>
+    <t>years_sponsorship</t>
+  </si>
+  <si>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -402,7 +408,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -410,17 +416,200 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -735,33 +924,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6A4B67E-A70E-FF47-86DD-9BF22E85C9FF}">
-  <dimension ref="A1:P97"/>
+  <dimension ref="A1:R97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" customWidth="1"/>
-    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:18" ht="17" thickBot="1">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>110</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -773,1172 +966,1962 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
         <v>16</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I1" t="s">
+        <v>108</v>
+      </c>
+      <c r="J1" t="s">
         <v>17</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" t="s">
+        <v>101</v>
+      </c>
+      <c r="M1" t="s">
+        <v>102</v>
+      </c>
+      <c r="N1" t="s">
+        <v>103</v>
+      </c>
+      <c r="O1" t="s">
+        <v>104</v>
+      </c>
+      <c r="P1" t="s">
         <v>106</v>
       </c>
-      <c r="I1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K1" t="s">
-        <v>102</v>
-      </c>
-      <c r="L1" t="s">
-        <v>103</v>
-      </c>
-      <c r="M1" t="s">
-        <v>104</v>
-      </c>
-      <c r="N1" t="s">
-        <v>105</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
+        <v>109</v>
+      </c>
+      <c r="R1" t="s">
         <v>107</v>
       </c>
-      <c r="P1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16">
-      <c r="A2">
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="7">
         <v>2023</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="8">
         <v>15</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="7">
         <v>13.65</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="7">
         <v>0</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="7">
         <v>0</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="7">
         <v>0</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="7">
+        <v>0</v>
+      </c>
+      <c r="J2" s="7">
         <f>E2+F2+G2+H2</f>
         <v>13.65</v>
       </c>
-      <c r="J2" s="1">
-        <f>I2-D2</f>
+      <c r="K2" s="8">
+        <f>J2-D2</f>
         <v>-1.3499999999999996</v>
       </c>
-      <c r="K2">
+      <c r="L2" s="7">
         <v>2023</v>
       </c>
-      <c r="L2">
+      <c r="M2" s="7">
         <f>SUM(E2:E13)</f>
-        <v>187.62</v>
-      </c>
-      <c r="M2">
+        <v>241.82</v>
+      </c>
+      <c r="N2" s="7">
         <f>SUM(F2:F13)</f>
         <v>4.93</v>
       </c>
-      <c r="N2">
+      <c r="O2" s="7">
         <f>SUM(G2:G13)</f>
         <v>38</v>
       </c>
-      <c r="O2">
+      <c r="P2" s="7">
         <f>SUM(H2:H13)</f>
         <v>250</v>
       </c>
-      <c r="P2">
-        <f>SUM(I2:I13)</f>
-        <v>480.55000000000007</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
-      <c r="A3">
+      <c r="Q2" s="7">
+        <v>0</v>
+      </c>
+      <c r="R2" s="9">
+        <f>SUM(J2:J13)</f>
+        <v>534.75000000000011</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3" s="10">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="11">
         <v>2023</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="12">
         <f>D2*1.1</f>
         <v>16.5</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="11">
         <v>23.92</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="11">
         <v>4.93</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="11">
         <v>0</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="11">
         <v>0</v>
       </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I13" si="0">E3+F3+G3+H3</f>
+      <c r="I3" s="18">
+        <v>0</v>
+      </c>
+      <c r="J3" s="11">
+        <f t="shared" ref="J3:J10" si="0">E3+F3+G3+H3</f>
         <v>28.85</v>
       </c>
-      <c r="J3" s="1">
-        <f t="shared" ref="J3:J4" si="1">I3-D3</f>
+      <c r="K3" s="12">
+        <f t="shared" ref="K3:K4" si="1">J3-D3</f>
         <v>12.350000000000001</v>
       </c>
-      <c r="K3">
+      <c r="L3" s="11">
         <v>2024</v>
       </c>
-    </row>
-    <row r="4" spans="1:16">
-      <c r="A4">
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="13"/>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4" s="10">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="11">
         <v>2023</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="12">
         <f>D3*1.1</f>
         <v>18.150000000000002</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="11">
         <v>23.52</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="11">
         <v>0</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="11">
         <v>0</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="11">
         <v>0</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="18">
+        <v>0</v>
+      </c>
+      <c r="J4" s="11">
         <f t="shared" si="0"/>
         <v>23.52</v>
       </c>
-      <c r="J4" s="1">
+      <c r="K4" s="12">
         <f t="shared" si="1"/>
         <v>5.3699999999999974</v>
       </c>
-    </row>
-    <row r="5" spans="1:16">
-      <c r="A5">
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="13"/>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" s="10">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="11">
         <v>2023</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="12">
         <f>D4*1.1</f>
         <v>19.965000000000003</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="11">
         <v>24.69</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="11">
         <v>0</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="11">
         <v>19</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="11">
         <v>0</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="18">
+        <v>0</v>
+      </c>
+      <c r="J5" s="11">
         <f t="shared" si="0"/>
         <v>43.69</v>
       </c>
-      <c r="J5" s="1">
-        <f>I5-D5</f>
+      <c r="K5" s="12">
+        <f>J5-D5</f>
         <v>23.724999999999994</v>
       </c>
-    </row>
-    <row r="6" spans="1:16">
-      <c r="A6">
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="13"/>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" s="10">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="11">
         <v>2023</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="12">
         <f t="shared" ref="D6:D69" si="2">D5*1.1</f>
         <v>21.961500000000004</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="11">
         <v>25.88</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="11">
         <v>0</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="11">
         <v>0</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="11">
         <v>0</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="18">
+        <v>0</v>
+      </c>
+      <c r="J6" s="11">
         <f t="shared" si="0"/>
         <v>25.88</v>
       </c>
-      <c r="J6" s="1">
-        <f>I6-D6</f>
+      <c r="K6" s="12">
+        <f>J6-D6</f>
         <v>3.9184999999999945</v>
       </c>
-    </row>
-    <row r="7" spans="1:16">
-      <c r="A7">
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="13"/>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7" s="10">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="11">
         <v>2023</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="12">
         <f t="shared" si="2"/>
         <v>24.157650000000007</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="11">
         <v>22.77</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="11">
         <v>0</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="11">
         <v>9.5</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="11">
         <v>250</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="18">
+        <v>0</v>
+      </c>
+      <c r="J7" s="11">
         <f t="shared" si="0"/>
         <v>282.27</v>
       </c>
-      <c r="J7" s="1">
-        <f>I7-D7</f>
+      <c r="K7" s="12">
+        <f>J7-D7</f>
         <v>258.11234999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:16">
-      <c r="A8">
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="13"/>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" s="10">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="11">
         <v>2023</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="12">
         <f t="shared" si="2"/>
         <v>26.573415000000011</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="11">
         <v>35.22</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="11">
         <v>0</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="11">
         <v>0</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="11">
         <v>0</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="18">
+        <v>0</v>
+      </c>
+      <c r="J8" s="11">
         <f t="shared" si="0"/>
         <v>35.22</v>
       </c>
-      <c r="J8" s="1">
-        <f t="shared" ref="J8:J13" si="3">I8-D8</f>
+      <c r="K8" s="12">
+        <f t="shared" ref="K8:K13" si="3">J8-D8</f>
         <v>8.6465849999999875</v>
       </c>
-    </row>
-    <row r="9" spans="1:16">
-      <c r="A9">
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="13"/>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9" s="10">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="11">
         <v>2023</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="12">
         <f t="shared" si="2"/>
         <v>29.230756500000016</v>
       </c>
-      <c r="E9">
-        <v>17.97</v>
-      </c>
-      <c r="F9">
+      <c r="E9" s="11">
+        <v>44.85</v>
+      </c>
+      <c r="F9" s="11">
         <v>0</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="11">
         <v>9.5</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="11">
         <v>0</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="18">
+        <v>0</v>
+      </c>
+      <c r="J9" s="11">
         <f t="shared" si="0"/>
-        <v>27.47</v>
-      </c>
-      <c r="J9" s="1">
+        <v>54.35</v>
+      </c>
+      <c r="K9" s="12">
         <f t="shared" si="3"/>
-        <v>-1.7607565000000172</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16">
-      <c r="A10">
+        <v>25.119243499999985</v>
+      </c>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="13"/>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="A10" s="10">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="11">
         <v>2023</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="12">
         <f t="shared" si="2"/>
         <v>32.153832150000021</v>
       </c>
-      <c r="F10">
+      <c r="E10" s="18">
+        <v>27.32</v>
+      </c>
+      <c r="F10" s="18">
         <v>0</v>
       </c>
-      <c r="I10">
+      <c r="G10" s="18">
+        <v>0</v>
+      </c>
+      <c r="H10" s="18">
+        <v>0</v>
+      </c>
+      <c r="I10" s="18">
+        <v>0</v>
+      </c>
+      <c r="J10" s="18">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J10" s="1">
+        <v>27.32</v>
+      </c>
+      <c r="K10" s="12">
         <f t="shared" si="3"/>
-        <v>-32.153832150000021</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16">
-      <c r="A11">
+        <v>-4.8338321500000205</v>
+      </c>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="13"/>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11" s="10">
         <v>10</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="11">
         <v>2023</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="12">
         <f t="shared" si="2"/>
         <v>35.369215365000024</v>
       </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J11" s="1">
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="12">
         <f t="shared" si="3"/>
         <v>-35.369215365000024</v>
       </c>
-    </row>
-    <row r="12" spans="1:16">
-      <c r="A12">
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="13"/>
+    </row>
+    <row r="12" spans="1:18">
+      <c r="A12" s="10">
         <v>11</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="11">
         <v>2023</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="12">
         <f t="shared" si="2"/>
         <v>38.906136901500027</v>
       </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J12" s="1">
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="18"/>
+      <c r="I12" s="18"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="12">
         <f t="shared" si="3"/>
         <v>-38.906136901500027</v>
       </c>
-    </row>
-    <row r="13" spans="1:16">
-      <c r="A13">
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="11"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="11"/>
+      <c r="R12" s="13"/>
+    </row>
+    <row r="13" spans="1:18" ht="17" thickBot="1">
+      <c r="A13" s="14">
         <v>12</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="15">
         <v>2023</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="16">
         <f t="shared" si="2"/>
         <v>42.796750591650031</v>
       </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J13" s="1">
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="16">
         <f t="shared" si="3"/>
         <v>-42.796750591650031</v>
       </c>
-    </row>
-    <row r="14" spans="1:16">
-      <c r="A14">
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+      <c r="P13" s="15"/>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="17"/>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="A14" s="6">
         <v>13</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="7">
         <v>2024</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="8">
         <f t="shared" si="2"/>
         <v>47.07642565081504</v>
       </c>
-    </row>
-    <row r="15" spans="1:16">
-      <c r="A15">
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="7"/>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="9"/>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="A15" s="10">
         <v>14</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="11">
         <v>2024</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="12">
         <f t="shared" si="2"/>
         <v>51.784068215896546</v>
       </c>
-    </row>
-    <row r="16" spans="1:16">
-      <c r="A16">
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="11"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11"/>
+      <c r="R15" s="13"/>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="A16" s="10">
         <v>15</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="11">
         <v>2024</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="12">
         <f t="shared" si="2"/>
         <v>56.962475037486207</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17">
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
+      <c r="O16" s="11"/>
+      <c r="P16" s="11"/>
+      <c r="Q16" s="11"/>
+      <c r="R16" s="13"/>
+    </row>
+    <row r="17" spans="1:18">
+      <c r="A17" s="10">
         <v>16</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="11">
         <v>2024</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="12">
         <f t="shared" si="2"/>
         <v>62.65872254123483</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18">
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="11"/>
+      <c r="O17" s="11"/>
+      <c r="P17" s="11"/>
+      <c r="Q17" s="11"/>
+      <c r="R17" s="13"/>
+    </row>
+    <row r="18" spans="1:18">
+      <c r="A18" s="10">
         <v>17</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="11">
         <v>2024</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18" s="12">
         <f t="shared" si="2"/>
         <v>68.924594795358317</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19">
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+      <c r="O18" s="11"/>
+      <c r="P18" s="11"/>
+      <c r="Q18" s="11"/>
+      <c r="R18" s="13"/>
+    </row>
+    <row r="19" spans="1:18">
+      <c r="A19" s="10">
         <v>18</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="11">
         <v>2024</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19" s="12">
         <f t="shared" si="2"/>
         <v>75.817054274894161</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20">
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
+      <c r="O19" s="11"/>
+      <c r="P19" s="11"/>
+      <c r="Q19" s="11"/>
+      <c r="R19" s="13"/>
+    </row>
+    <row r="20" spans="1:18">
+      <c r="A20" s="10">
         <v>19</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="11">
         <v>2024</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20" s="12">
         <f t="shared" si="2"/>
         <v>83.398759702383586</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21">
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+      <c r="O20" s="11"/>
+      <c r="P20" s="11"/>
+      <c r="Q20" s="11"/>
+      <c r="R20" s="13"/>
+    </row>
+    <row r="21" spans="1:18">
+      <c r="A21" s="10">
         <v>20</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="11">
         <v>2024</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" s="12">
         <f t="shared" si="2"/>
         <v>91.738635672621953</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22">
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+      <c r="O21" s="11"/>
+      <c r="P21" s="11"/>
+      <c r="Q21" s="11"/>
+      <c r="R21" s="13"/>
+    </row>
+    <row r="22" spans="1:18">
+      <c r="A22" s="10">
         <v>21</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="11">
         <v>2024</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22" s="12">
         <f t="shared" si="2"/>
         <v>100.91249923988416</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23">
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="11"/>
+      <c r="P22" s="11"/>
+      <c r="Q22" s="11"/>
+      <c r="R22" s="13"/>
+    </row>
+    <row r="23" spans="1:18">
+      <c r="A23" s="10">
         <v>22</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="11">
         <v>2024</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D23" s="12">
         <f t="shared" si="2"/>
         <v>111.00374916387258</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24">
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11"/>
+      <c r="M23" s="11"/>
+      <c r="N23" s="11"/>
+      <c r="O23" s="11"/>
+      <c r="P23" s="11"/>
+      <c r="Q23" s="11"/>
+      <c r="R23" s="13"/>
+    </row>
+    <row r="24" spans="1:18">
+      <c r="A24" s="10">
         <v>23</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="11">
         <v>2024</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D24" s="12">
         <f t="shared" si="2"/>
         <v>122.10412408025985</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25">
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
+      <c r="O24" s="11"/>
+      <c r="P24" s="11"/>
+      <c r="Q24" s="11"/>
+      <c r="R24" s="13"/>
+    </row>
+    <row r="25" spans="1:18" ht="17" thickBot="1">
+      <c r="A25" s="14">
         <v>24</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="15">
         <v>2024</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D25" s="16">
         <f t="shared" si="2"/>
         <v>134.31453648828585</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26">
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="15"/>
+      <c r="L25" s="15"/>
+      <c r="M25" s="15"/>
+      <c r="N25" s="15"/>
+      <c r="O25" s="15"/>
+      <c r="P25" s="15"/>
+      <c r="Q25" s="15"/>
+      <c r="R25" s="17"/>
+    </row>
+    <row r="26" spans="1:18">
+      <c r="A26" s="6">
         <v>25</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="7">
         <v>2025</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D26" s="8">
         <f t="shared" si="2"/>
         <v>147.74599013711446</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27">
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="7"/>
+      <c r="P26" s="7"/>
+      <c r="Q26" s="7"/>
+      <c r="R26" s="9"/>
+    </row>
+    <row r="27" spans="1:18">
+      <c r="A27" s="10">
         <v>26</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="11">
         <v>2025</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D27" s="12">
         <f t="shared" si="2"/>
         <v>162.52058915082591</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28">
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="11"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="11"/>
+      <c r="M27" s="11"/>
+      <c r="N27" s="11"/>
+      <c r="O27" s="11"/>
+      <c r="P27" s="11"/>
+      <c r="Q27" s="11"/>
+      <c r="R27" s="13"/>
+    </row>
+    <row r="28" spans="1:18">
+      <c r="A28" s="10">
         <v>27</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="11">
         <v>2025</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D28" s="12">
         <f t="shared" si="2"/>
         <v>178.77264806590853</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29">
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="11"/>
+      <c r="N28" s="11"/>
+      <c r="O28" s="11"/>
+      <c r="P28" s="11"/>
+      <c r="Q28" s="11"/>
+      <c r="R28" s="13"/>
+    </row>
+    <row r="29" spans="1:18">
+      <c r="A29" s="10">
         <v>28</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="11">
         <v>2025</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D29" s="12">
         <f t="shared" si="2"/>
         <v>196.64991287249939</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30">
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="11"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="11"/>
+      <c r="K29" s="11"/>
+      <c r="L29" s="11"/>
+      <c r="M29" s="11"/>
+      <c r="N29" s="11"/>
+      <c r="O29" s="11"/>
+      <c r="P29" s="11"/>
+      <c r="Q29" s="11"/>
+      <c r="R29" s="13"/>
+    </row>
+    <row r="30" spans="1:18">
+      <c r="A30" s="10">
         <v>29</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="11">
         <v>2025</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D30" s="12">
         <f t="shared" si="2"/>
         <v>216.31490415974935</v>
       </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31">
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="11"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="11"/>
+      <c r="K30" s="11"/>
+      <c r="L30" s="11"/>
+      <c r="M30" s="11"/>
+      <c r="N30" s="11"/>
+      <c r="O30" s="11"/>
+      <c r="P30" s="11"/>
+      <c r="Q30" s="11"/>
+      <c r="R30" s="13"/>
+    </row>
+    <row r="31" spans="1:18">
+      <c r="A31" s="10">
         <v>30</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="11">
         <v>2025</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D31" s="1">
+      <c r="D31" s="12">
         <f t="shared" si="2"/>
         <v>237.9463945757243</v>
       </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32">
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="11"/>
+      <c r="M31" s="11"/>
+      <c r="N31" s="11"/>
+      <c r="O31" s="11"/>
+      <c r="P31" s="11"/>
+      <c r="Q31" s="11"/>
+      <c r="R31" s="13"/>
+    </row>
+    <row r="32" spans="1:18">
+      <c r="A32" s="10">
         <v>31</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="11">
         <v>2025</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D32" s="1">
+      <c r="D32" s="12">
         <f t="shared" si="2"/>
         <v>261.74103403329673</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33">
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="H32" s="11"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="11"/>
+      <c r="K32" s="11"/>
+      <c r="L32" s="11"/>
+      <c r="M32" s="11"/>
+      <c r="N32" s="11"/>
+      <c r="O32" s="11"/>
+      <c r="P32" s="11"/>
+      <c r="Q32" s="11"/>
+      <c r="R32" s="13"/>
+    </row>
+    <row r="33" spans="1:18">
+      <c r="A33" s="10">
         <v>32</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="11">
         <v>2025</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D33" s="1">
+      <c r="D33" s="12">
         <f t="shared" si="2"/>
         <v>287.91513743662642</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34">
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+      <c r="I33" s="11"/>
+      <c r="J33" s="11"/>
+      <c r="K33" s="11"/>
+      <c r="L33" s="11"/>
+      <c r="M33" s="11"/>
+      <c r="N33" s="11"/>
+      <c r="O33" s="11"/>
+      <c r="P33" s="11"/>
+      <c r="Q33" s="11"/>
+      <c r="R33" s="13"/>
+    </row>
+    <row r="34" spans="1:18">
+      <c r="A34" s="10">
         <v>33</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="11">
         <v>2025</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D34" s="1">
+      <c r="D34" s="12">
         <f t="shared" si="2"/>
         <v>316.7066511802891</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35">
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="H34" s="11"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="11"/>
+      <c r="K34" s="11"/>
+      <c r="L34" s="11"/>
+      <c r="M34" s="11"/>
+      <c r="N34" s="11"/>
+      <c r="O34" s="11"/>
+      <c r="P34" s="11"/>
+      <c r="Q34" s="11"/>
+      <c r="R34" s="13"/>
+    </row>
+    <row r="35" spans="1:18">
+      <c r="A35" s="10">
         <v>34</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="11">
         <v>2025</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D35" s="1">
+      <c r="D35" s="12">
         <f t="shared" si="2"/>
         <v>348.37731629831802</v>
       </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36">
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="11"/>
+      <c r="J35" s="11"/>
+      <c r="K35" s="11"/>
+      <c r="L35" s="11"/>
+      <c r="M35" s="11"/>
+      <c r="N35" s="11"/>
+      <c r="O35" s="11"/>
+      <c r="P35" s="11"/>
+      <c r="Q35" s="11"/>
+      <c r="R35" s="13"/>
+    </row>
+    <row r="36" spans="1:18">
+      <c r="A36" s="10">
         <v>35</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="11">
         <v>2025</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D36" s="1">
+      <c r="D36" s="12">
         <f t="shared" si="2"/>
         <v>383.21504792814983</v>
       </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37">
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="11"/>
+      <c r="J36" s="11"/>
+      <c r="K36" s="11"/>
+      <c r="L36" s="11"/>
+      <c r="M36" s="11"/>
+      <c r="N36" s="11"/>
+      <c r="O36" s="11"/>
+      <c r="P36" s="11"/>
+      <c r="Q36" s="11"/>
+      <c r="R36" s="13"/>
+    </row>
+    <row r="37" spans="1:18">
+      <c r="A37" s="10">
         <v>36</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="11">
         <v>2025</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D37" s="1">
+      <c r="D37" s="12">
         <f t="shared" si="2"/>
         <v>421.53655272096483</v>
       </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38">
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="11"/>
+      <c r="I37" s="11"/>
+      <c r="J37" s="11"/>
+      <c r="K37" s="11"/>
+      <c r="L37" s="11"/>
+      <c r="M37" s="11"/>
+      <c r="N37" s="11"/>
+      <c r="O37" s="11"/>
+      <c r="P37" s="11"/>
+      <c r="Q37" s="11"/>
+      <c r="R37" s="13"/>
+    </row>
+    <row r="38" spans="1:18">
+      <c r="A38" s="19">
         <v>37</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="20">
         <v>2026</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="D38" s="1">
+      <c r="D38" s="21">
         <f t="shared" si="2"/>
         <v>463.69020799306134</v>
       </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39">
+      <c r="E38" s="20"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="20"/>
+      <c r="I38" s="20"/>
+      <c r="J38" s="20"/>
+      <c r="K38" s="20"/>
+      <c r="L38" s="20"/>
+      <c r="M38" s="20"/>
+      <c r="N38" s="20"/>
+      <c r="O38" s="20"/>
+      <c r="P38" s="20"/>
+      <c r="Q38" s="20"/>
+      <c r="R38" s="22"/>
+    </row>
+    <row r="39" spans="1:18">
+      <c r="A39" s="23">
         <v>38</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="11">
         <v>2026</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D39" s="1">
+      <c r="D39" s="12">
         <f t="shared" si="2"/>
         <v>510.05922879236749</v>
       </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40">
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
+      <c r="I39" s="11"/>
+      <c r="J39" s="11"/>
+      <c r="K39" s="11"/>
+      <c r="L39" s="11"/>
+      <c r="M39" s="11"/>
+      <c r="N39" s="11"/>
+      <c r="O39" s="11"/>
+      <c r="P39" s="11"/>
+      <c r="Q39" s="11"/>
+      <c r="R39" s="24"/>
+    </row>
+    <row r="40" spans="1:18">
+      <c r="A40" s="23">
         <v>39</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="11">
         <v>2026</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D40" s="1">
+      <c r="D40" s="12">
         <f t="shared" si="2"/>
         <v>561.06515167160433</v>
       </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41">
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="11"/>
+      <c r="I40" s="11"/>
+      <c r="J40" s="11"/>
+      <c r="K40" s="11"/>
+      <c r="L40" s="11"/>
+      <c r="M40" s="11"/>
+      <c r="N40" s="11"/>
+      <c r="O40" s="11"/>
+      <c r="P40" s="11"/>
+      <c r="Q40" s="11"/>
+      <c r="R40" s="24"/>
+    </row>
+    <row r="41" spans="1:18">
+      <c r="A41" s="23">
         <v>40</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="11">
         <v>2026</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D41" s="1">
+      <c r="D41" s="12">
         <f t="shared" si="2"/>
         <v>617.17166683876485</v>
       </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42">
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="11"/>
+      <c r="J41" s="11"/>
+      <c r="K41" s="11"/>
+      <c r="L41" s="11"/>
+      <c r="M41" s="11"/>
+      <c r="N41" s="11"/>
+      <c r="O41" s="11"/>
+      <c r="P41" s="11"/>
+      <c r="Q41" s="11"/>
+      <c r="R41" s="24"/>
+    </row>
+    <row r="42" spans="1:18">
+      <c r="A42" s="23">
         <v>41</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="11">
         <v>2026</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D42" s="1">
+      <c r="D42" s="12">
         <f t="shared" si="2"/>
         <v>678.88883352264133</v>
       </c>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43">
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="11"/>
+      <c r="H42" s="11"/>
+      <c r="I42" s="11"/>
+      <c r="J42" s="11"/>
+      <c r="K42" s="11"/>
+      <c r="L42" s="11"/>
+      <c r="M42" s="11"/>
+      <c r="N42" s="11"/>
+      <c r="O42" s="11"/>
+      <c r="P42" s="11"/>
+      <c r="Q42" s="11"/>
+      <c r="R42" s="24"/>
+    </row>
+    <row r="43" spans="1:18">
+      <c r="A43" s="23">
         <v>42</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="11">
         <v>2026</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D43" s="1">
+      <c r="D43" s="12">
         <f t="shared" si="2"/>
         <v>746.77771687490554</v>
       </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44">
+      <c r="E43" s="11"/>
+      <c r="F43" s="11"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="11"/>
+      <c r="I43" s="11"/>
+      <c r="J43" s="11"/>
+      <c r="K43" s="11"/>
+      <c r="L43" s="11"/>
+      <c r="M43" s="11"/>
+      <c r="N43" s="11"/>
+      <c r="O43" s="11"/>
+      <c r="P43" s="11"/>
+      <c r="Q43" s="11"/>
+      <c r="R43" s="24"/>
+    </row>
+    <row r="44" spans="1:18">
+      <c r="A44" s="23">
         <v>43</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="11">
         <v>2026</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D44" s="1">
+      <c r="D44" s="12">
         <f t="shared" si="2"/>
         <v>821.45548856239611</v>
       </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45">
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="11"/>
+      <c r="H44" s="11"/>
+      <c r="I44" s="11"/>
+      <c r="J44" s="11"/>
+      <c r="K44" s="11"/>
+      <c r="L44" s="11"/>
+      <c r="M44" s="11"/>
+      <c r="N44" s="11"/>
+      <c r="O44" s="11"/>
+      <c r="P44" s="11"/>
+      <c r="Q44" s="11"/>
+      <c r="R44" s="24"/>
+    </row>
+    <row r="45" spans="1:18">
+      <c r="A45" s="23">
         <v>44</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="11">
         <v>2026</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D45" s="1">
+      <c r="D45" s="12">
         <f t="shared" si="2"/>
         <v>903.60103741863577</v>
       </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46">
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="11"/>
+      <c r="I45" s="11"/>
+      <c r="J45" s="11"/>
+      <c r="K45" s="11"/>
+      <c r="L45" s="11"/>
+      <c r="M45" s="11"/>
+      <c r="N45" s="11"/>
+      <c r="O45" s="11"/>
+      <c r="P45" s="11"/>
+      <c r="Q45" s="11"/>
+      <c r="R45" s="24"/>
+    </row>
+    <row r="46" spans="1:18">
+      <c r="A46" s="23">
         <v>45</v>
       </c>
-      <c r="B46">
+      <c r="B46" s="11">
         <v>2026</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D46" s="1">
+      <c r="D46" s="12">
         <f t="shared" si="2"/>
         <v>993.96114116049944</v>
       </c>
-    </row>
-    <row r="47" spans="1:4">
-      <c r="A47">
+      <c r="E46" s="11"/>
+      <c r="F46" s="11"/>
+      <c r="G46" s="11"/>
+      <c r="H46" s="11"/>
+      <c r="I46" s="11"/>
+      <c r="J46" s="11"/>
+      <c r="K46" s="11"/>
+      <c r="L46" s="11"/>
+      <c r="M46" s="11"/>
+      <c r="N46" s="11"/>
+      <c r="O46" s="11"/>
+      <c r="P46" s="11"/>
+      <c r="Q46" s="11"/>
+      <c r="R46" s="24"/>
+    </row>
+    <row r="47" spans="1:18">
+      <c r="A47" s="23">
         <v>46</v>
       </c>
-      <c r="B47">
+      <c r="B47" s="11">
         <v>2026</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D47" s="1">
+      <c r="D47" s="12">
         <f t="shared" si="2"/>
         <v>1093.3572552765495</v>
       </c>
-    </row>
-    <row r="48" spans="1:4">
-      <c r="A48">
+      <c r="E47" s="11"/>
+      <c r="F47" s="11"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="11"/>
+      <c r="J47" s="11"/>
+      <c r="K47" s="11"/>
+      <c r="L47" s="11"/>
+      <c r="M47" s="11"/>
+      <c r="N47" s="11"/>
+      <c r="O47" s="11"/>
+      <c r="P47" s="11"/>
+      <c r="Q47" s="11"/>
+      <c r="R47" s="24"/>
+    </row>
+    <row r="48" spans="1:18">
+      <c r="A48" s="23">
         <v>47</v>
       </c>
-      <c r="B48">
+      <c r="B48" s="11">
         <v>2026</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D48" s="1">
+      <c r="D48" s="12">
         <f t="shared" si="2"/>
         <v>1202.6929808042046</v>
       </c>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="A49">
+      <c r="E48" s="11"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="11"/>
+      <c r="H48" s="11"/>
+      <c r="I48" s="11"/>
+      <c r="J48" s="11"/>
+      <c r="K48" s="11"/>
+      <c r="L48" s="11"/>
+      <c r="M48" s="11"/>
+      <c r="N48" s="11"/>
+      <c r="O48" s="11"/>
+      <c r="P48" s="11"/>
+      <c r="Q48" s="11"/>
+      <c r="R48" s="24"/>
+    </row>
+    <row r="49" spans="1:18">
+      <c r="A49" s="25">
         <v>48</v>
       </c>
-      <c r="B49">
+      <c r="B49" s="26">
         <v>2026</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="D49" s="1">
+      <c r="D49" s="27">
         <f t="shared" si="2"/>
         <v>1322.9622788846252</v>
       </c>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="A50">
+      <c r="E49" s="26"/>
+      <c r="F49" s="26"/>
+      <c r="G49" s="26"/>
+      <c r="H49" s="26"/>
+      <c r="I49" s="26"/>
+      <c r="J49" s="26"/>
+      <c r="K49" s="26"/>
+      <c r="L49" s="26"/>
+      <c r="M49" s="26"/>
+      <c r="N49" s="26"/>
+      <c r="O49" s="26"/>
+      <c r="P49" s="26"/>
+      <c r="Q49" s="26"/>
+      <c r="R49" s="28"/>
+    </row>
+    <row r="50" spans="1:18">
+      <c r="A50" s="19">
         <v>49</v>
       </c>
-      <c r="B50">
+      <c r="B50" s="20">
         <v>2027</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="D50" s="1">
+      <c r="D50" s="21">
         <f t="shared" si="2"/>
         <v>1455.2585067730879</v>
       </c>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="A51">
+      <c r="E50" s="20"/>
+      <c r="F50" s="20"/>
+      <c r="G50" s="20"/>
+      <c r="H50" s="20"/>
+      <c r="I50" s="20"/>
+      <c r="J50" s="20"/>
+      <c r="K50" s="20"/>
+      <c r="L50" s="20"/>
+      <c r="M50" s="20"/>
+      <c r="N50" s="20"/>
+      <c r="O50" s="20"/>
+      <c r="P50" s="20"/>
+      <c r="Q50" s="20"/>
+      <c r="R50" s="22"/>
+    </row>
+    <row r="51" spans="1:18">
+      <c r="A51" s="23">
         <v>50</v>
       </c>
-      <c r="B51">
+      <c r="B51" s="11">
         <v>2027</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D51" s="1">
+      <c r="D51" s="12">
         <f t="shared" si="2"/>
         <v>1600.7843574503968</v>
       </c>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52">
+      <c r="E51" s="11"/>
+      <c r="F51" s="11"/>
+      <c r="G51" s="11"/>
+      <c r="H51" s="11"/>
+      <c r="I51" s="11"/>
+      <c r="J51" s="11"/>
+      <c r="K51" s="11"/>
+      <c r="L51" s="11"/>
+      <c r="M51" s="11"/>
+      <c r="N51" s="11"/>
+      <c r="O51" s="11"/>
+      <c r="P51" s="11"/>
+      <c r="Q51" s="11"/>
+      <c r="R51" s="24"/>
+    </row>
+    <row r="52" spans="1:18">
+      <c r="A52" s="23">
         <v>51</v>
       </c>
-      <c r="B52">
+      <c r="B52" s="11">
         <v>2027</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D52" s="1">
+      <c r="D52" s="12">
         <f t="shared" si="2"/>
         <v>1760.8627931954366</v>
       </c>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="A53">
+      <c r="E52" s="11"/>
+      <c r="F52" s="11"/>
+      <c r="G52" s="11"/>
+      <c r="H52" s="11"/>
+      <c r="I52" s="11"/>
+      <c r="J52" s="11"/>
+      <c r="K52" s="11"/>
+      <c r="L52" s="11"/>
+      <c r="M52" s="11"/>
+      <c r="N52" s="11"/>
+      <c r="O52" s="11"/>
+      <c r="P52" s="11"/>
+      <c r="Q52" s="11"/>
+      <c r="R52" s="24"/>
+    </row>
+    <row r="53" spans="1:18">
+      <c r="A53" s="23">
         <v>52</v>
       </c>
-      <c r="B53">
+      <c r="B53" s="11">
         <v>2027</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D53" s="1">
+      <c r="D53" s="12">
         <f t="shared" si="2"/>
         <v>1936.9490725149803</v>
       </c>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54">
+      <c r="E53" s="11"/>
+      <c r="F53" s="11"/>
+      <c r="G53" s="11"/>
+      <c r="H53" s="11"/>
+      <c r="I53" s="11"/>
+      <c r="J53" s="11"/>
+      <c r="K53" s="11"/>
+      <c r="L53" s="11"/>
+      <c r="M53" s="11"/>
+      <c r="N53" s="11"/>
+      <c r="O53" s="11"/>
+      <c r="P53" s="11"/>
+      <c r="Q53" s="11"/>
+      <c r="R53" s="24"/>
+    </row>
+    <row r="54" spans="1:18">
+      <c r="A54" s="23">
         <v>53</v>
       </c>
-      <c r="B54">
+      <c r="B54" s="11">
         <v>2027</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D54" s="1">
+      <c r="D54" s="12">
         <f t="shared" si="2"/>
         <v>2130.6439797664784</v>
       </c>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55">
+      <c r="E54" s="11"/>
+      <c r="F54" s="11"/>
+      <c r="G54" s="11"/>
+      <c r="H54" s="11"/>
+      <c r="I54" s="11"/>
+      <c r="J54" s="11"/>
+      <c r="K54" s="11"/>
+      <c r="L54" s="11"/>
+      <c r="M54" s="11"/>
+      <c r="N54" s="11"/>
+      <c r="O54" s="11"/>
+      <c r="P54" s="11"/>
+      <c r="Q54" s="11"/>
+      <c r="R54" s="24"/>
+    </row>
+    <row r="55" spans="1:18">
+      <c r="A55" s="23">
         <v>54</v>
       </c>
-      <c r="B55">
+      <c r="B55" s="11">
         <v>2027</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D55" s="1">
+      <c r="D55" s="12">
         <f t="shared" si="2"/>
         <v>2343.7083777431267</v>
       </c>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56">
+      <c r="E55" s="11"/>
+      <c r="F55" s="11"/>
+      <c r="G55" s="11"/>
+      <c r="H55" s="11"/>
+      <c r="I55" s="11"/>
+      <c r="J55" s="11"/>
+      <c r="K55" s="11"/>
+      <c r="L55" s="11"/>
+      <c r="M55" s="11"/>
+      <c r="N55" s="11"/>
+      <c r="O55" s="11"/>
+      <c r="P55" s="11"/>
+      <c r="Q55" s="11"/>
+      <c r="R55" s="24"/>
+    </row>
+    <row r="56" spans="1:18">
+      <c r="A56" s="23">
         <v>55</v>
       </c>
-      <c r="B56">
+      <c r="B56" s="11">
         <v>2027</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="D56" s="1">
+      <c r="D56" s="12">
         <f t="shared" si="2"/>
         <v>2578.0792155174395</v>
       </c>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57">
+      <c r="E56" s="11"/>
+      <c r="F56" s="11"/>
+      <c r="G56" s="11"/>
+      <c r="H56" s="11"/>
+      <c r="I56" s="11"/>
+      <c r="J56" s="11"/>
+      <c r="K56" s="11"/>
+      <c r="L56" s="11"/>
+      <c r="M56" s="11"/>
+      <c r="N56" s="11"/>
+      <c r="O56" s="11"/>
+      <c r="P56" s="11"/>
+      <c r="Q56" s="11"/>
+      <c r="R56" s="24"/>
+    </row>
+    <row r="57" spans="1:18">
+      <c r="A57" s="23">
         <v>56</v>
       </c>
-      <c r="B57">
+      <c r="B57" s="11">
         <v>2027</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D57" s="1">
+      <c r="D57" s="12">
         <f t="shared" si="2"/>
         <v>2835.8871370691836</v>
       </c>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58">
+      <c r="E57" s="11"/>
+      <c r="F57" s="11"/>
+      <c r="G57" s="11"/>
+      <c r="H57" s="11"/>
+      <c r="I57" s="11"/>
+      <c r="J57" s="11"/>
+      <c r="K57" s="11"/>
+      <c r="L57" s="11"/>
+      <c r="M57" s="11"/>
+      <c r="N57" s="11"/>
+      <c r="O57" s="11"/>
+      <c r="P57" s="11"/>
+      <c r="Q57" s="11"/>
+      <c r="R57" s="24"/>
+    </row>
+    <row r="58" spans="1:18">
+      <c r="A58" s="23">
         <v>57</v>
       </c>
-      <c r="B58">
+      <c r="B58" s="11">
         <v>2027</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="D58" s="1">
+      <c r="D58" s="12">
         <f t="shared" si="2"/>
         <v>3119.4758507761021</v>
       </c>
-    </row>
-    <row r="59" spans="1:4">
-      <c r="A59">
+      <c r="E58" s="11"/>
+      <c r="F58" s="11"/>
+      <c r="G58" s="11"/>
+      <c r="H58" s="11"/>
+      <c r="I58" s="11"/>
+      <c r="J58" s="11"/>
+      <c r="K58" s="11"/>
+      <c r="L58" s="11"/>
+      <c r="M58" s="11"/>
+      <c r="N58" s="11"/>
+      <c r="O58" s="11"/>
+      <c r="P58" s="11"/>
+      <c r="Q58" s="11"/>
+      <c r="R58" s="24"/>
+    </row>
+    <row r="59" spans="1:18">
+      <c r="A59" s="23">
         <v>58</v>
       </c>
-      <c r="B59">
+      <c r="B59" s="11">
         <v>2027</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="D59" s="1">
+      <c r="D59" s="12">
         <f t="shared" si="2"/>
         <v>3431.4234358537128</v>
       </c>
-    </row>
-    <row r="60" spans="1:4">
-      <c r="A60">
+      <c r="E59" s="11"/>
+      <c r="F59" s="11"/>
+      <c r="G59" s="11"/>
+      <c r="H59" s="11"/>
+      <c r="I59" s="11"/>
+      <c r="J59" s="11"/>
+      <c r="K59" s="11"/>
+      <c r="L59" s="11"/>
+      <c r="M59" s="11"/>
+      <c r="N59" s="11"/>
+      <c r="O59" s="11"/>
+      <c r="P59" s="11"/>
+      <c r="Q59" s="11"/>
+      <c r="R59" s="24"/>
+    </row>
+    <row r="60" spans="1:18">
+      <c r="A60" s="23">
         <v>59</v>
       </c>
-      <c r="B60">
+      <c r="B60" s="11">
         <v>2027</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D60" s="1">
+      <c r="D60" s="12">
         <f t="shared" si="2"/>
         <v>3774.5657794390845</v>
       </c>
-    </row>
-    <row r="61" spans="1:4">
-      <c r="A61">
+      <c r="E60" s="11"/>
+      <c r="F60" s="11"/>
+      <c r="G60" s="11"/>
+      <c r="H60" s="11"/>
+      <c r="I60" s="11"/>
+      <c r="J60" s="11"/>
+      <c r="K60" s="11"/>
+      <c r="L60" s="11"/>
+      <c r="M60" s="11"/>
+      <c r="N60" s="11"/>
+      <c r="O60" s="11"/>
+      <c r="P60" s="11"/>
+      <c r="Q60" s="11"/>
+      <c r="R60" s="24"/>
+    </row>
+    <row r="61" spans="1:18">
+      <c r="A61" s="25">
         <v>60</v>
       </c>
-      <c r="B61">
+      <c r="B61" s="26">
         <v>2027</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="D61" s="1">
+      <c r="D61" s="27">
         <f t="shared" si="2"/>
         <v>4152.0223573829935</v>
       </c>
-    </row>
-    <row r="62" spans="1:4">
+      <c r="E61" s="26"/>
+      <c r="F61" s="26"/>
+      <c r="G61" s="26"/>
+      <c r="H61" s="26"/>
+      <c r="I61" s="26"/>
+      <c r="J61" s="26"/>
+      <c r="K61" s="26"/>
+      <c r="L61" s="26"/>
+      <c r="M61" s="26"/>
+      <c r="N61" s="26"/>
+      <c r="O61" s="26"/>
+      <c r="P61" s="26"/>
+      <c r="Q61" s="26"/>
+      <c r="R61" s="28"/>
+    </row>
+    <row r="62" spans="1:18">
       <c r="A62">
         <v>61</v>
       </c>
@@ -1953,7 +2936,7 @@
         <v>4567.2245931212929</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:18">
       <c r="A63">
         <v>62</v>
       </c>
@@ -1968,7 +2951,7 @@
         <v>5023.9470524334229</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:18">
       <c r="A64">
         <v>63</v>
       </c>
@@ -2502,461 +3485,461 @@
   <sheetData>
     <row r="1" spans="1:5" ht="17">
       <c r="A1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="18">
       <c r="A2" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="4">
         <v>823</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="18">
       <c r="A3" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3" s="4">
         <v>301</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="17">
       <c r="A4" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4" s="5">
         <v>246</v>
       </c>
       <c r="C4" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>36</v>
-      </c>
       <c r="E4" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="17">
       <c r="A5" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B5" s="5">
         <v>246</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>36</v>
-      </c>
       <c r="E5" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="17">
       <c r="A6" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6" s="5">
         <v>135</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>40</v>
-      </c>
       <c r="E6" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="18">
       <c r="A7" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" s="4">
         <v>110</v>
       </c>
       <c r="C7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>43</v>
-      </c>
       <c r="E7" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="17">
       <c r="A8" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="5">
         <v>110</v>
       </c>
       <c r="C8" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>46</v>
-      </c>
       <c r="E8" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="17">
       <c r="A9" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B9" s="5">
         <v>110</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>46</v>
-      </c>
       <c r="E9" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="17">
       <c r="A10" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B10" s="5">
         <v>110</v>
       </c>
       <c r="C10" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>50</v>
-      </c>
       <c r="E10" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="17">
       <c r="A11" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B11" s="5">
         <v>90.5</v>
       </c>
       <c r="C11" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>53</v>
-      </c>
       <c r="E11" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="17">
       <c r="A12" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B12" s="5">
         <v>74</v>
       </c>
       <c r="C12" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>56</v>
-      </c>
       <c r="E12" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="17">
       <c r="A13" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B13" s="5">
         <v>60.5</v>
       </c>
       <c r="C13" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>59</v>
-      </c>
       <c r="E13" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="17">
       <c r="A14" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B14" s="5">
         <v>60.5</v>
       </c>
       <c r="C14" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>62</v>
-      </c>
       <c r="E14" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="17">
       <c r="A15" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B15" s="5">
         <v>49.5</v>
       </c>
       <c r="C15" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>65</v>
-      </c>
       <c r="E15" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="17">
       <c r="A16" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B16" s="5">
         <v>33.1</v>
       </c>
       <c r="C16" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>68</v>
-      </c>
       <c r="E16" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="17">
       <c r="A17" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B17" s="5">
         <v>33.1</v>
       </c>
       <c r="C17" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>71</v>
-      </c>
       <c r="E17" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="17">
       <c r="A18" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B18" s="5">
         <v>27.1</v>
       </c>
       <c r="C18" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>74</v>
-      </c>
       <c r="E18" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="17">
       <c r="A19" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B19" s="5">
         <v>27.1</v>
       </c>
       <c r="C19" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="D19" s="5" t="s">
-        <v>77</v>
-      </c>
       <c r="E19" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="17">
       <c r="A20" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B20" s="5">
         <v>27.1</v>
       </c>
       <c r="C20" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>80</v>
-      </c>
       <c r="E20" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="17">
       <c r="A21" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B21" s="5">
         <v>9.9</v>
       </c>
       <c r="C21" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D21" s="5" t="s">
-        <v>83</v>
-      </c>
       <c r="E21" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="17">
       <c r="A22" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B22" s="5">
         <v>6.6</v>
       </c>
       <c r="C22" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>86</v>
-      </c>
       <c r="E22" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="17">
       <c r="A23" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B23" s="5">
         <v>6.6</v>
       </c>
       <c r="C23" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D23" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="D23" s="5" t="s">
-        <v>89</v>
-      </c>
       <c r="E23" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="17">
       <c r="A24" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B24" s="5">
         <v>5.4</v>
       </c>
       <c r="C24" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D24" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="D24" s="5" t="s">
-        <v>92</v>
-      </c>
       <c r="E24" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="17">
       <c r="A25" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B25" s="5">
         <v>5.4</v>
       </c>
       <c r="C25" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D25" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="D25" s="5" t="s">
-        <v>95</v>
-      </c>
       <c r="E25" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="17">
       <c r="A26" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B26" s="5">
         <v>4.4000000000000004</v>
       </c>
       <c r="C26" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D26" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>98</v>
-      </c>
       <c r="E26" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="17">
       <c r="A27" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B27" s="5">
         <v>4.4000000000000004</v>
       </c>
       <c r="C27" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="D27" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="D27" s="5" t="s">
-        <v>101</v>
-      </c>
       <c r="E27" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
glmulti link for the video works, wenn I knit the blog post, but does not work, when I build the whole website
</commit_message>
<xml_diff>
--- a/_site/compounding_growth_10_percent.xlsx
+++ b/_site/compounding_growth_10_percent.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zablotski/Library/Mobile Documents/com~apple~CloudDocs/7. Hobby/programming and stats/yuzaR-Blog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{508A28C7-8583-9240-A3D9-7A8695F64164}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60DEB8D7-8020-114F-A0F0-BCFA4C755B09}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{EDD741CF-9DB9-2945-BF15-255A1807DC69}"/>
   </bookViews>
@@ -927,7 +927,7 @@
   <dimension ref="A1:R97"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1049,7 +1049,7 @@
       </c>
       <c r="M2" s="7">
         <f>SUM(E2:E13)</f>
-        <v>297.93</v>
+        <v>303.48</v>
       </c>
       <c r="N2" s="7">
         <f>SUM(F2:F13)</f>
@@ -1068,7 +1068,7 @@
       </c>
       <c r="R2" s="9">
         <f>SUM(J2:J13)</f>
-        <v>590.86</v>
+        <v>596.41000000000008</v>
       </c>
     </row>
     <row r="3" spans="1:18">
@@ -1448,7 +1448,7 @@
         <v>35.369215365000024</v>
       </c>
       <c r="E11" s="18">
-        <v>37.79</v>
+        <v>43.34</v>
       </c>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
@@ -1456,11 +1456,11 @@
       <c r="I11" s="18"/>
       <c r="J11" s="18">
         <f t="shared" si="0"/>
-        <v>37.79</v>
+        <v>43.34</v>
       </c>
       <c r="K11" s="12">
         <f t="shared" si="3"/>
-        <v>2.4207846349999755</v>
+        <v>7.9707846349999798</v>
       </c>
       <c r="L11" s="11"/>
       <c r="M11" s="11"/>

</xml_diff>

<commit_message>
neu try from new mac
</commit_message>
<xml_diff>
--- a/_site/compounding_growth_10_percent.xlsx
+++ b/_site/compounding_growth_10_percent.xlsx
@@ -1,32 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zablotski/Library/Mobile Documents/com~apple~CloudDocs/7. Hobby/programming and stats/yuzaR-Blog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60DEB8D7-8020-114F-A0F0-BCFA4C755B09}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CA4CE6C-BC0C-FF4D-B2A7-01313168F1BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{EDD741CF-9DB9-2945-BF15-255A1807DC69}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="33600" windowHeight="20060" xr2:uid="{EDD741CF-9DB9-2945-BF15-255A1807DC69}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="keywords" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="113">
   <si>
     <t>year</t>
   </si>
@@ -359,6 +370,12 @@
   </si>
   <si>
     <t>id</t>
+  </si>
+  <si>
+    <t>years_total_projected</t>
+  </si>
+  <si>
+    <t>YOY GROWTH</t>
   </si>
 </sst>
 </file>
@@ -592,14 +609,11 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -610,6 +624,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" indent="4"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -625,6 +646,1080 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>projected</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$2:$D$16</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18.150000000000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19.965000000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21.961500000000004</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24.157650000000007</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>26.573415000000011</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>29.230756500000016</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>32.153832150000021</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>35.369215365000024</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>38.906136901500027</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>42.796750591650031</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>47.07642565081504</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>51.784068215896546</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>56.962475037486207</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F6BA-7E42-89D9-89C6F9BFA471}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>adds</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>13.65</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>23.92</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.52</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24.69</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25.88</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22.77</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>35.22</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>44.85</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45.64</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>49.56</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>63.76</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>48.01</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>42.62</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F6BA-7E42-89D9-89C6F9BFA471}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="1629692688"/>
+        <c:axId val="1629694368"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1629692688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1629694368"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1629694368"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1629692688"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>141110</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>79374</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>670276</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>176388</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D72DAF49-DC16-B24F-9279-1C482C09AA3C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -924,10 +2019,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6A4B67E-A70E-FF47-86DD-9BF22E85C9FF}">
-  <dimension ref="A1:R97"/>
+  <dimension ref="A1:T97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -950,65 +2045,73 @@
     <col min="16" max="16" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="17" thickBot="1">
-      <c r="A1" t="s">
+    <row r="1" spans="1:20" ht="17" thickBot="1">
+      <c r="A1" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="9" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="2" spans="1:18">
+      <c r="S1" t="s">
+        <v>111</v>
+      </c>
+      <c r="T1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" ht="17" thickBot="1">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -1049,7 +2152,7 @@
       </c>
       <c r="M2" s="7">
         <f>SUM(E2:E13)</f>
-        <v>303.48</v>
+        <v>421.46999999999997</v>
       </c>
       <c r="N2" s="7">
         <f>SUM(F2:F13)</f>
@@ -1068,479 +2171,504 @@
       </c>
       <c r="R2" s="9">
         <f>SUM(J2:J13)</f>
-        <v>596.41000000000008</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18">
+        <v>714.40000000000009</v>
+      </c>
+      <c r="S2" s="27">
+        <f>SUM(D2:D13)</f>
+        <v>320.76425650815014</v>
+      </c>
+      <c r="T2" s="28">
+        <f>(S3*100)/S2</f>
+        <v>313.84283767210036</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
       <c r="A3" s="10">
         <v>2</v>
       </c>
-      <c r="B3" s="11">
+      <c r="B3">
         <v>2023</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="1">
         <f>D2*1.1</f>
         <v>16.5</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3">
         <v>23.92</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3">
         <v>4.93</v>
       </c>
-      <c r="G3" s="11">
-        <v>0</v>
-      </c>
-      <c r="H3" s="11">
-        <v>0</v>
-      </c>
-      <c r="I3" s="18">
-        <v>0</v>
-      </c>
-      <c r="J3" s="11">
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
         <f t="shared" ref="J3:J13" si="0">E3+F3+G3+H3</f>
         <v>28.85</v>
       </c>
-      <c r="K3" s="12">
+      <c r="K3" s="1">
         <f t="shared" ref="K3:K4" si="1">J3-D3</f>
         <v>12.350000000000001</v>
       </c>
-      <c r="L3" s="11">
+      <c r="L3">
         <v>2024</v>
       </c>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
-      <c r="P3" s="11"/>
-      <c r="Q3" s="11"/>
-      <c r="R3" s="13"/>
-    </row>
-    <row r="4" spans="1:18">
+      <c r="M3" s="7">
+        <f>SUM(E14:E25)</f>
+        <v>42.62</v>
+      </c>
+      <c r="N3" s="7">
+        <f t="shared" ref="N3:R3" si="2">SUM(F14:F25)</f>
+        <v>0</v>
+      </c>
+      <c r="O3" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P3" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q3" s="7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R3" s="9">
+        <f t="shared" si="2"/>
+        <v>42.62</v>
+      </c>
+      <c r="S3" s="27">
+        <f>SUM(D14:D25)</f>
+        <v>1006.6956448629932</v>
+      </c>
+      <c r="T3" s="27">
+        <f t="shared" ref="T3:T4" si="3">(S4*100)/S3</f>
+        <v>313.8428376721003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
       <c r="A4" s="10">
         <v>3</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4">
         <v>2023</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="1">
         <f>D3*1.1</f>
         <v>18.150000000000002</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4">
         <v>23.52</v>
       </c>
-      <c r="F4" s="11">
-        <v>0</v>
-      </c>
-      <c r="G4" s="11">
-        <v>0</v>
-      </c>
-      <c r="H4" s="11">
-        <v>0</v>
-      </c>
-      <c r="I4" s="18">
-        <v>0</v>
-      </c>
-      <c r="J4" s="11">
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
         <f t="shared" si="0"/>
         <v>23.52</v>
       </c>
-      <c r="K4" s="12">
+      <c r="K4" s="1">
         <f t="shared" si="1"/>
         <v>5.3699999999999974</v>
       </c>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="13"/>
-    </row>
-    <row r="5" spans="1:18">
+      <c r="R4" s="11"/>
+      <c r="S4" s="27">
+        <f>SUM(D26:D37)</f>
+        <v>3159.4421785594668</v>
+      </c>
+      <c r="T4" s="27">
+        <f t="shared" si="3"/>
+        <v>313.84283767210019</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
       <c r="A5" s="10">
         <v>4</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5">
         <v>2023</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="1">
         <f>D4*1.1</f>
         <v>19.965000000000003</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5">
         <v>24.69</v>
       </c>
-      <c r="F5" s="11">
-        <v>0</v>
-      </c>
-      <c r="G5" s="11">
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
         <v>19</v>
       </c>
-      <c r="H5" s="11">
-        <v>0</v>
-      </c>
-      <c r="I5" s="18">
-        <v>0</v>
-      </c>
-      <c r="J5" s="11">
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
         <f t="shared" si="0"/>
         <v>43.69</v>
       </c>
-      <c r="K5" s="12">
+      <c r="K5" s="1">
         <f>J5-D5</f>
         <v>23.724999999999994</v>
       </c>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="11"/>
-      <c r="O5" s="11"/>
-      <c r="P5" s="11"/>
-      <c r="Q5" s="11"/>
-      <c r="R5" s="13"/>
-    </row>
-    <row r="6" spans="1:18">
+      <c r="R5" s="11"/>
+      <c r="S5" s="27">
+        <f>SUM(D38:D49)</f>
+        <v>9915.6829878002536</v>
+      </c>
+      <c r="T5" s="26"/>
+    </row>
+    <row r="6" spans="1:20">
       <c r="A6" s="10">
         <v>5</v>
       </c>
-      <c r="B6" s="11">
+      <c r="B6">
         <v>2023</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="12">
-        <f t="shared" ref="D6:D69" si="2">D5*1.1</f>
+      <c r="D6" s="1">
+        <f t="shared" ref="D6:D69" si="4">D5*1.1</f>
         <v>21.961500000000004</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6">
         <v>25.88</v>
       </c>
-      <c r="F6" s="11">
-        <v>0</v>
-      </c>
-      <c r="G6" s="11">
-        <v>0</v>
-      </c>
-      <c r="H6" s="11">
-        <v>0</v>
-      </c>
-      <c r="I6" s="18">
-        <v>0</v>
-      </c>
-      <c r="J6" s="11">
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
         <f t="shared" si="0"/>
         <v>25.88</v>
       </c>
-      <c r="K6" s="12">
+      <c r="K6" s="1">
         <f>J6-D6</f>
         <v>3.9184999999999945</v>
       </c>
-      <c r="L6" s="11"/>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="11"/>
-      <c r="P6" s="11"/>
-      <c r="Q6" s="11"/>
-      <c r="R6" s="13"/>
-    </row>
-    <row r="7" spans="1:18">
+      <c r="R6" s="11"/>
+      <c r="S6" s="27">
+        <f>SUM(D50:D61)</f>
+        <v>31119.66086348203</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20">
       <c r="A7" s="10">
         <v>6</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7">
         <v>2023</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="12">
-        <f t="shared" si="2"/>
+      <c r="D7" s="1">
+        <f t="shared" si="4"/>
         <v>24.157650000000007</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7">
         <v>22.77</v>
       </c>
-      <c r="F7" s="11">
-        <v>0</v>
-      </c>
-      <c r="G7" s="11">
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
         <v>9.5</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H7">
         <v>250</v>
       </c>
-      <c r="I7" s="18">
-        <v>0</v>
-      </c>
-      <c r="J7" s="11">
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
         <f t="shared" si="0"/>
         <v>282.27</v>
       </c>
-      <c r="K7" s="12">
+      <c r="K7" s="1">
         <f>J7-D7</f>
         <v>258.11234999999999</v>
       </c>
-      <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
-      <c r="N7" s="11"/>
-      <c r="O7" s="11"/>
-      <c r="P7" s="11"/>
-      <c r="Q7" s="11"/>
-      <c r="R7" s="13"/>
-    </row>
-    <row r="8" spans="1:18">
+      <c r="R7" s="11"/>
+    </row>
+    <row r="8" spans="1:20">
       <c r="A8" s="10">
         <v>7</v>
       </c>
-      <c r="B8" s="11">
+      <c r="B8">
         <v>2023</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="12">
-        <f t="shared" si="2"/>
+      <c r="D8" s="1">
+        <f t="shared" si="4"/>
         <v>26.573415000000011</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8">
         <v>35.22</v>
       </c>
-      <c r="F8" s="11">
-        <v>0</v>
-      </c>
-      <c r="G8" s="11">
-        <v>0</v>
-      </c>
-      <c r="H8" s="11">
-        <v>0</v>
-      </c>
-      <c r="I8" s="18">
-        <v>0</v>
-      </c>
-      <c r="J8" s="11">
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
         <f t="shared" si="0"/>
         <v>35.22</v>
       </c>
-      <c r="K8" s="12">
-        <f t="shared" ref="K8:K13" si="3">J8-D8</f>
+      <c r="K8" s="1">
+        <f t="shared" ref="K8:K13" si="5">J8-D8</f>
         <v>8.6465849999999875</v>
       </c>
-      <c r="L8" s="11"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="11"/>
-      <c r="O8" s="11"/>
-      <c r="P8" s="11"/>
-      <c r="Q8" s="11"/>
-      <c r="R8" s="13"/>
-    </row>
-    <row r="9" spans="1:18">
+      <c r="R8" s="11"/>
+    </row>
+    <row r="9" spans="1:20">
       <c r="A9" s="10">
         <v>8</v>
       </c>
-      <c r="B9" s="11">
+      <c r="B9">
         <v>2023</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="12">
-        <f t="shared" si="2"/>
+      <c r="D9" s="1">
+        <f t="shared" si="4"/>
         <v>29.230756500000016</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9">
         <v>44.85</v>
       </c>
-      <c r="F9" s="11">
-        <v>0</v>
-      </c>
-      <c r="G9" s="11">
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
         <v>9.5</v>
       </c>
-      <c r="H9" s="11">
-        <v>0</v>
-      </c>
-      <c r="I9" s="18">
-        <v>0</v>
-      </c>
-      <c r="J9" s="11">
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
         <f t="shared" si="0"/>
         <v>54.35</v>
       </c>
-      <c r="K9" s="12">
-        <f t="shared" si="3"/>
+      <c r="K9" s="1">
+        <f t="shared" si="5"/>
         <v>25.119243499999985</v>
       </c>
-      <c r="L9" s="11"/>
-      <c r="M9" s="11"/>
-      <c r="N9" s="11"/>
-      <c r="O9" s="11"/>
-      <c r="P9" s="11"/>
-      <c r="Q9" s="11"/>
-      <c r="R9" s="13"/>
-    </row>
-    <row r="10" spans="1:18">
+      <c r="R9" s="11"/>
+    </row>
+    <row r="10" spans="1:20">
       <c r="A10" s="10">
         <v>9</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B10">
         <v>2023</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="12">
-        <f t="shared" si="2"/>
+      <c r="D10" s="1">
+        <f t="shared" si="4"/>
         <v>32.153832150000021</v>
       </c>
-      <c r="E10" s="18">
+      <c r="E10">
         <v>45.64</v>
       </c>
-      <c r="F10" s="18">
-        <v>0</v>
-      </c>
-      <c r="G10" s="18">
-        <v>0</v>
-      </c>
-      <c r="H10" s="18">
-        <v>0</v>
-      </c>
-      <c r="I10" s="18">
-        <v>0</v>
-      </c>
-      <c r="J10" s="18">
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
         <f t="shared" si="0"/>
         <v>45.64</v>
       </c>
-      <c r="K10" s="12">
-        <f t="shared" si="3"/>
+      <c r="K10" s="1">
+        <f t="shared" si="5"/>
         <v>13.48616784999998</v>
       </c>
-      <c r="L10" s="11"/>
-      <c r="M10" s="11"/>
-      <c r="N10" s="11"/>
-      <c r="O10" s="11"/>
-      <c r="P10" s="11"/>
-      <c r="Q10" s="11"/>
-      <c r="R10" s="13"/>
-    </row>
-    <row r="11" spans="1:18">
+      <c r="R10" s="11"/>
+    </row>
+    <row r="11" spans="1:20">
       <c r="A11" s="10">
         <v>10</v>
       </c>
-      <c r="B11" s="11">
+      <c r="B11">
         <v>2023</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="12">
-        <f t="shared" si="2"/>
+      <c r="D11" s="1">
+        <f t="shared" si="4"/>
         <v>35.369215365000024</v>
       </c>
-      <c r="E11" s="18">
-        <v>43.34</v>
-      </c>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="18"/>
-      <c r="I11" s="18"/>
-      <c r="J11" s="18">
+      <c r="E11">
+        <v>49.56</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
         <f t="shared" si="0"/>
-        <v>43.34</v>
-      </c>
-      <c r="K11" s="12">
-        <f t="shared" si="3"/>
-        <v>7.9707846349999798</v>
-      </c>
-      <c r="L11" s="11"/>
-      <c r="M11" s="11"/>
-      <c r="N11" s="11"/>
-      <c r="O11" s="11"/>
-      <c r="P11" s="11"/>
-      <c r="Q11" s="11"/>
-      <c r="R11" s="13"/>
-    </row>
-    <row r="12" spans="1:18">
+        <v>49.56</v>
+      </c>
+      <c r="K11" s="1">
+        <f t="shared" si="5"/>
+        <v>14.190784634999979</v>
+      </c>
+      <c r="R11" s="11"/>
+    </row>
+    <row r="12" spans="1:20">
       <c r="A12" s="10">
         <v>11</v>
       </c>
-      <c r="B12" s="11">
+      <c r="B12">
         <v>2023</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="12">
-        <f t="shared" si="2"/>
+      <c r="D12" s="1">
+        <f t="shared" si="4"/>
         <v>38.906136901500027</v>
       </c>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="18"/>
-      <c r="J12" s="18">
+      <c r="E12">
+        <v>63.76</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K12" s="12">
-        <f t="shared" si="3"/>
-        <v>-38.906136901500027</v>
-      </c>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
-      <c r="N12" s="11"/>
-      <c r="O12" s="11"/>
-      <c r="P12" s="11"/>
-      <c r="Q12" s="11"/>
-      <c r="R12" s="13"/>
-    </row>
-    <row r="13" spans="1:18" ht="17" thickBot="1">
-      <c r="A13" s="14">
+        <v>63.76</v>
+      </c>
+      <c r="K12" s="1">
+        <f t="shared" si="5"/>
+        <v>24.853863098499971</v>
+      </c>
+      <c r="R12" s="11"/>
+    </row>
+    <row r="13" spans="1:20" ht="17" thickBot="1">
+      <c r="A13" s="12">
         <v>12</v>
       </c>
-      <c r="B13" s="15">
+      <c r="B13" s="13">
         <v>2023</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="16">
-        <f t="shared" si="2"/>
+      <c r="D13" s="14">
+        <f t="shared" si="4"/>
         <v>42.796750591650031</v>
       </c>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="18">
+      <c r="E13" s="13">
+        <v>48.01</v>
+      </c>
+      <c r="F13" s="13">
+        <v>0</v>
+      </c>
+      <c r="G13" s="13">
+        <v>0</v>
+      </c>
+      <c r="H13" s="13">
+        <v>0</v>
+      </c>
+      <c r="I13" s="13">
+        <v>0</v>
+      </c>
+      <c r="J13" s="13">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K13" s="16">
-        <f t="shared" si="3"/>
-        <v>-42.796750591650031</v>
-      </c>
-      <c r="L13" s="15"/>
-      <c r="M13" s="15"/>
-      <c r="N13" s="15"/>
-      <c r="O13" s="15"/>
-      <c r="P13" s="15"/>
-      <c r="Q13" s="15"/>
-      <c r="R13" s="17"/>
-    </row>
-    <row r="14" spans="1:18">
+        <v>48.01</v>
+      </c>
+      <c r="K13" s="14">
+        <f t="shared" si="5"/>
+        <v>5.2132494083499665</v>
+      </c>
+      <c r="L13" s="13"/>
+      <c r="M13" s="13"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="13"/>
+      <c r="P13" s="13"/>
+      <c r="Q13" s="13"/>
+      <c r="R13" s="15"/>
+    </row>
+    <row r="14" spans="1:20">
       <c r="A14" s="6">
         <v>13</v>
       </c>
@@ -1551,16 +2679,32 @@
         <v>3</v>
       </c>
       <c r="D14" s="8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>47.07642565081504</v>
       </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
-      <c r="K14" s="7"/>
+      <c r="E14" s="7">
+        <v>42.62</v>
+      </c>
+      <c r="F14" s="7">
+        <v>0</v>
+      </c>
+      <c r="G14" s="7">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <f t="shared" ref="J14:J25" si="6">E14+F14+G14+H14</f>
+        <v>42.62</v>
+      </c>
+      <c r="K14" s="8">
+        <f t="shared" ref="K14:K25" si="7">J14-D14</f>
+        <v>-4.4564256508150422</v>
+      </c>
       <c r="L14" s="7"/>
       <c r="M14" s="7"/>
       <c r="N14" s="7"/>
@@ -1569,346 +2713,423 @@
       <c r="Q14" s="7"/>
       <c r="R14" s="9"/>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:20">
       <c r="A15" s="10">
         <v>14</v>
       </c>
-      <c r="B15" s="11">
+      <c r="B15">
         <v>2024</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" t="s">
         <v>4</v>
       </c>
-      <c r="D15" s="12">
-        <f t="shared" si="2"/>
+      <c r="D15" s="1">
+        <f t="shared" si="4"/>
         <v>51.784068215896546</v>
       </c>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11"/>
-      <c r="N15" s="11"/>
-      <c r="O15" s="11"/>
-      <c r="P15" s="11"/>
-      <c r="Q15" s="11"/>
-      <c r="R15" s="13"/>
-    </row>
-    <row r="16" spans="1:18">
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K15" s="1">
+        <f t="shared" si="7"/>
+        <v>-51.784068215896546</v>
+      </c>
+      <c r="R15" s="11"/>
+    </row>
+    <row r="16" spans="1:20">
       <c r="A16" s="10">
         <v>15</v>
       </c>
-      <c r="B16" s="11">
+      <c r="B16">
         <v>2024</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="12">
-        <f t="shared" si="2"/>
+      <c r="D16" s="1">
+        <f t="shared" si="4"/>
         <v>56.962475037486207</v>
       </c>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="11"/>
-      <c r="N16" s="11"/>
-      <c r="O16" s="11"/>
-      <c r="P16" s="11"/>
-      <c r="Q16" s="11"/>
-      <c r="R16" s="13"/>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K16" s="1">
+        <f t="shared" si="7"/>
+        <v>-56.962475037486207</v>
+      </c>
+      <c r="R16" s="11"/>
     </row>
     <row r="17" spans="1:18">
       <c r="A17" s="10">
         <v>16</v>
       </c>
-      <c r="B17" s="11">
+      <c r="B17">
         <v>2024</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="12">
-        <f t="shared" si="2"/>
+      <c r="D17" s="1">
+        <f t="shared" si="4"/>
         <v>62.65872254123483</v>
       </c>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="11"/>
-      <c r="M17" s="11"/>
-      <c r="N17" s="11"/>
-      <c r="O17" s="11"/>
-      <c r="P17" s="11"/>
-      <c r="Q17" s="11"/>
-      <c r="R17" s="13"/>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K17" s="1">
+        <f t="shared" si="7"/>
+        <v>-62.65872254123483</v>
+      </c>
+      <c r="R17" s="11"/>
     </row>
     <row r="18" spans="1:18">
       <c r="A18" s="10">
         <v>17</v>
       </c>
-      <c r="B18" s="11">
+      <c r="B18">
         <v>2024</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="12">
-        <f t="shared" si="2"/>
+      <c r="D18" s="1">
+        <f t="shared" si="4"/>
         <v>68.924594795358317</v>
       </c>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="11"/>
-      <c r="L18" s="11"/>
-      <c r="M18" s="11"/>
-      <c r="N18" s="11"/>
-      <c r="O18" s="11"/>
-      <c r="P18" s="11"/>
-      <c r="Q18" s="11"/>
-      <c r="R18" s="13"/>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K18" s="1">
+        <f t="shared" si="7"/>
+        <v>-68.924594795358317</v>
+      </c>
+      <c r="R18" s="11"/>
     </row>
     <row r="19" spans="1:18">
       <c r="A19" s="10">
         <v>18</v>
       </c>
-      <c r="B19" s="11">
+      <c r="B19">
         <v>2024</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="12">
-        <f t="shared" si="2"/>
+      <c r="D19" s="1">
+        <f t="shared" si="4"/>
         <v>75.817054274894161</v>
       </c>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="11"/>
-      <c r="M19" s="11"/>
-      <c r="N19" s="11"/>
-      <c r="O19" s="11"/>
-      <c r="P19" s="11"/>
-      <c r="Q19" s="11"/>
-      <c r="R19" s="13"/>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K19" s="1">
+        <f t="shared" si="7"/>
+        <v>-75.817054274894161</v>
+      </c>
+      <c r="R19" s="11"/>
     </row>
     <row r="20" spans="1:18">
       <c r="A20" s="10">
         <v>19</v>
       </c>
-      <c r="B20" s="11">
+      <c r="B20">
         <v>2024</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="12">
-        <f t="shared" si="2"/>
+      <c r="D20" s="1">
+        <f t="shared" si="4"/>
         <v>83.398759702383586</v>
       </c>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="11"/>
-      <c r="L20" s="11"/>
-      <c r="M20" s="11"/>
-      <c r="N20" s="11"/>
-      <c r="O20" s="11"/>
-      <c r="P20" s="11"/>
-      <c r="Q20" s="11"/>
-      <c r="R20" s="13"/>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K20" s="1">
+        <f t="shared" si="7"/>
+        <v>-83.398759702383586</v>
+      </c>
+      <c r="R20" s="11"/>
     </row>
     <row r="21" spans="1:18">
       <c r="A21" s="10">
         <v>20</v>
       </c>
-      <c r="B21" s="11">
+      <c r="B21">
         <v>2024</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="12">
-        <f t="shared" si="2"/>
+      <c r="D21" s="1">
+        <f t="shared" si="4"/>
         <v>91.738635672621953</v>
       </c>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="11"/>
-      <c r="L21" s="11"/>
-      <c r="M21" s="11"/>
-      <c r="N21" s="11"/>
-      <c r="O21" s="11"/>
-      <c r="P21" s="11"/>
-      <c r="Q21" s="11"/>
-      <c r="R21" s="13"/>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K21" s="1">
+        <f t="shared" si="7"/>
+        <v>-91.738635672621953</v>
+      </c>
+      <c r="R21" s="11"/>
     </row>
     <row r="22" spans="1:18">
       <c r="A22" s="10">
         <v>21</v>
       </c>
-      <c r="B22" s="11">
+      <c r="B22">
         <v>2024</v>
       </c>
-      <c r="C22" s="11" t="s">
+      <c r="C22" t="s">
         <v>11</v>
       </c>
-      <c r="D22" s="12">
-        <f t="shared" si="2"/>
+      <c r="D22" s="1">
+        <f t="shared" si="4"/>
         <v>100.91249923988416</v>
       </c>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="11"/>
-      <c r="L22" s="11"/>
-      <c r="M22" s="11"/>
-      <c r="N22" s="11"/>
-      <c r="O22" s="11"/>
-      <c r="P22" s="11"/>
-      <c r="Q22" s="11"/>
-      <c r="R22" s="13"/>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K22" s="1">
+        <f t="shared" si="7"/>
+        <v>-100.91249923988416</v>
+      </c>
+      <c r="R22" s="11"/>
     </row>
     <row r="23" spans="1:18">
       <c r="A23" s="10">
         <v>22</v>
       </c>
-      <c r="B23" s="11">
+      <c r="B23">
         <v>2024</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="12">
-        <f t="shared" si="2"/>
+      <c r="D23" s="1">
+        <f t="shared" si="4"/>
         <v>111.00374916387258</v>
       </c>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="11"/>
-      <c r="L23" s="11"/>
-      <c r="M23" s="11"/>
-      <c r="N23" s="11"/>
-      <c r="O23" s="11"/>
-      <c r="P23" s="11"/>
-      <c r="Q23" s="11"/>
-      <c r="R23" s="13"/>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K23" s="1">
+        <f t="shared" si="7"/>
+        <v>-111.00374916387258</v>
+      </c>
+      <c r="R23" s="11"/>
     </row>
     <row r="24" spans="1:18">
       <c r="A24" s="10">
         <v>23</v>
       </c>
-      <c r="B24" s="11">
+      <c r="B24">
         <v>2024</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" t="s">
         <v>13</v>
       </c>
-      <c r="D24" s="12">
-        <f t="shared" si="2"/>
+      <c r="D24" s="1">
+        <f t="shared" si="4"/>
         <v>122.10412408025985</v>
       </c>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="11"/>
-      <c r="L24" s="11"/>
-      <c r="M24" s="11"/>
-      <c r="N24" s="11"/>
-      <c r="O24" s="11"/>
-      <c r="P24" s="11"/>
-      <c r="Q24" s="11"/>
-      <c r="R24" s="13"/>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K24" s="1">
+        <f t="shared" si="7"/>
+        <v>-122.10412408025985</v>
+      </c>
+      <c r="R24" s="11"/>
     </row>
     <row r="25" spans="1:18" ht="17" thickBot="1">
-      <c r="A25" s="14">
+      <c r="A25" s="12">
         <v>24</v>
       </c>
-      <c r="B25" s="15">
+      <c r="B25" s="13">
         <v>2024</v>
       </c>
-      <c r="C25" s="15" t="s">
+      <c r="C25" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D25" s="16">
-        <f t="shared" si="2"/>
+      <c r="D25" s="14">
+        <f t="shared" si="4"/>
         <v>134.31453648828585</v>
       </c>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="15"/>
-      <c r="I25" s="15"/>
-      <c r="J25" s="15"/>
-      <c r="K25" s="15"/>
-      <c r="L25" s="15"/>
-      <c r="M25" s="15"/>
-      <c r="N25" s="15"/>
-      <c r="O25" s="15"/>
-      <c r="P25" s="15"/>
-      <c r="Q25" s="15"/>
-      <c r="R25" s="17"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13">
+        <v>0</v>
+      </c>
+      <c r="G25" s="13">
+        <v>0</v>
+      </c>
+      <c r="H25" s="13">
+        <v>0</v>
+      </c>
+      <c r="I25" s="13">
+        <v>0</v>
+      </c>
+      <c r="J25" s="13">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K25" s="14">
+        <f t="shared" si="7"/>
+        <v>-134.31453648828585</v>
+      </c>
+      <c r="L25" s="13"/>
+      <c r="M25" s="13"/>
+      <c r="N25" s="13"/>
+      <c r="O25" s="13"/>
+      <c r="P25" s="13"/>
+      <c r="Q25" s="13"/>
+      <c r="R25" s="15"/>
     </row>
     <row r="26" spans="1:18">
-      <c r="A26" s="6">
+      <c r="A26" s="10">
         <v>25</v>
       </c>
-      <c r="B26" s="7">
+      <c r="B26">
         <v>2025</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" t="s">
         <v>3</v>
       </c>
-      <c r="D26" s="8">
-        <f t="shared" si="2"/>
+      <c r="D26" s="1">
+        <f t="shared" si="4"/>
         <v>147.74599013711446</v>
       </c>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="7"/>
-      <c r="I26" s="7"/>
-      <c r="J26" s="7"/>
-      <c r="K26" s="7"/>
       <c r="L26" s="7"/>
       <c r="M26" s="7"/>
       <c r="N26" s="7"/>
@@ -1921,1016 +3142,613 @@
       <c r="A27" s="10">
         <v>26</v>
       </c>
-      <c r="B27" s="11">
+      <c r="B27">
         <v>2025</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" t="s">
         <v>4</v>
       </c>
-      <c r="D27" s="12">
-        <f t="shared" si="2"/>
+      <c r="D27" s="1">
+        <f t="shared" si="4"/>
         <v>162.52058915082591</v>
       </c>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="11"/>
-      <c r="K27" s="11"/>
-      <c r="L27" s="11"/>
-      <c r="M27" s="11"/>
-      <c r="N27" s="11"/>
-      <c r="O27" s="11"/>
-      <c r="P27" s="11"/>
-      <c r="Q27" s="11"/>
-      <c r="R27" s="13"/>
+      <c r="R27" s="11"/>
     </row>
     <row r="28" spans="1:18">
       <c r="A28" s="10">
         <v>27</v>
       </c>
-      <c r="B28" s="11">
+      <c r="B28">
         <v>2025</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C28" t="s">
         <v>5</v>
       </c>
-      <c r="D28" s="12">
-        <f t="shared" si="2"/>
+      <c r="D28" s="1">
+        <f t="shared" si="4"/>
         <v>178.77264806590853</v>
       </c>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="11"/>
-      <c r="K28" s="11"/>
-      <c r="L28" s="11"/>
-      <c r="M28" s="11"/>
-      <c r="N28" s="11"/>
-      <c r="O28" s="11"/>
-      <c r="P28" s="11"/>
-      <c r="Q28" s="11"/>
-      <c r="R28" s="13"/>
+      <c r="R28" s="11"/>
     </row>
     <row r="29" spans="1:18">
       <c r="A29" s="10">
         <v>28</v>
       </c>
-      <c r="B29" s="11">
+      <c r="B29">
         <v>2025</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="C29" t="s">
         <v>6</v>
       </c>
-      <c r="D29" s="12">
-        <f t="shared" si="2"/>
+      <c r="D29" s="1">
+        <f t="shared" si="4"/>
         <v>196.64991287249939</v>
       </c>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="11"/>
-      <c r="K29" s="11"/>
-      <c r="L29" s="11"/>
-      <c r="M29" s="11"/>
-      <c r="N29" s="11"/>
-      <c r="O29" s="11"/>
-      <c r="P29" s="11"/>
-      <c r="Q29" s="11"/>
-      <c r="R29" s="13"/>
+      <c r="R29" s="11"/>
     </row>
     <row r="30" spans="1:18">
       <c r="A30" s="10">
         <v>29</v>
       </c>
-      <c r="B30" s="11">
+      <c r="B30">
         <v>2025</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="C30" t="s">
         <v>7</v>
       </c>
-      <c r="D30" s="12">
-        <f t="shared" si="2"/>
+      <c r="D30" s="1">
+        <f t="shared" si="4"/>
         <v>216.31490415974935</v>
       </c>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="11"/>
-      <c r="K30" s="11"/>
-      <c r="L30" s="11"/>
-      <c r="M30" s="11"/>
-      <c r="N30" s="11"/>
-      <c r="O30" s="11"/>
-      <c r="P30" s="11"/>
-      <c r="Q30" s="11"/>
-      <c r="R30" s="13"/>
+      <c r="R30" s="11"/>
     </row>
     <row r="31" spans="1:18">
       <c r="A31" s="10">
         <v>30</v>
       </c>
-      <c r="B31" s="11">
+      <c r="B31">
         <v>2025</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" t="s">
         <v>8</v>
       </c>
-      <c r="D31" s="12">
-        <f t="shared" si="2"/>
+      <c r="D31" s="1">
+        <f t="shared" si="4"/>
         <v>237.9463945757243</v>
       </c>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
-      <c r="I31" s="11"/>
-      <c r="J31" s="11"/>
-      <c r="K31" s="11"/>
-      <c r="L31" s="11"/>
-      <c r="M31" s="11"/>
-      <c r="N31" s="11"/>
-      <c r="O31" s="11"/>
-      <c r="P31" s="11"/>
-      <c r="Q31" s="11"/>
-      <c r="R31" s="13"/>
+      <c r="R31" s="11"/>
     </row>
     <row r="32" spans="1:18">
       <c r="A32" s="10">
         <v>31</v>
       </c>
-      <c r="B32" s="11">
+      <c r="B32">
         <v>2025</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C32" t="s">
         <v>9</v>
       </c>
-      <c r="D32" s="12">
-        <f t="shared" si="2"/>
+      <c r="D32" s="1">
+        <f t="shared" si="4"/>
         <v>261.74103403329673</v>
       </c>
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
-      <c r="I32" s="11"/>
-      <c r="J32" s="11"/>
-      <c r="K32" s="11"/>
-      <c r="L32" s="11"/>
-      <c r="M32" s="11"/>
-      <c r="N32" s="11"/>
-      <c r="O32" s="11"/>
-      <c r="P32" s="11"/>
-      <c r="Q32" s="11"/>
-      <c r="R32" s="13"/>
+      <c r="R32" s="11"/>
     </row>
     <row r="33" spans="1:18">
       <c r="A33" s="10">
         <v>32</v>
       </c>
-      <c r="B33" s="11">
+      <c r="B33">
         <v>2025</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="C33" t="s">
         <v>10</v>
       </c>
-      <c r="D33" s="12">
-        <f t="shared" si="2"/>
+      <c r="D33" s="1">
+        <f t="shared" si="4"/>
         <v>287.91513743662642</v>
       </c>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="11"/>
-      <c r="J33" s="11"/>
-      <c r="K33" s="11"/>
-      <c r="L33" s="11"/>
-      <c r="M33" s="11"/>
-      <c r="N33" s="11"/>
-      <c r="O33" s="11"/>
-      <c r="P33" s="11"/>
-      <c r="Q33" s="11"/>
-      <c r="R33" s="13"/>
+      <c r="R33" s="11"/>
     </row>
     <row r="34" spans="1:18">
       <c r="A34" s="10">
         <v>33</v>
       </c>
-      <c r="B34" s="11">
+      <c r="B34">
         <v>2025</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="C34" t="s">
         <v>11</v>
       </c>
-      <c r="D34" s="12">
-        <f t="shared" si="2"/>
+      <c r="D34" s="1">
+        <f t="shared" si="4"/>
         <v>316.7066511802891</v>
       </c>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="11"/>
-      <c r="J34" s="11"/>
-      <c r="K34" s="11"/>
-      <c r="L34" s="11"/>
-      <c r="M34" s="11"/>
-      <c r="N34" s="11"/>
-      <c r="O34" s="11"/>
-      <c r="P34" s="11"/>
-      <c r="Q34" s="11"/>
-      <c r="R34" s="13"/>
+      <c r="R34" s="11"/>
     </row>
     <row r="35" spans="1:18">
       <c r="A35" s="10">
         <v>34</v>
       </c>
-      <c r="B35" s="11">
+      <c r="B35">
         <v>2025</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C35" t="s">
         <v>12</v>
       </c>
-      <c r="D35" s="12">
-        <f t="shared" si="2"/>
+      <c r="D35" s="1">
+        <f t="shared" si="4"/>
         <v>348.37731629831802</v>
       </c>
-      <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="11"/>
-      <c r="I35" s="11"/>
-      <c r="J35" s="11"/>
-      <c r="K35" s="11"/>
-      <c r="L35" s="11"/>
-      <c r="M35" s="11"/>
-      <c r="N35" s="11"/>
-      <c r="O35" s="11"/>
-      <c r="P35" s="11"/>
-      <c r="Q35" s="11"/>
-      <c r="R35" s="13"/>
+      <c r="R35" s="11"/>
     </row>
     <row r="36" spans="1:18">
       <c r="A36" s="10">
         <v>35</v>
       </c>
-      <c r="B36" s="11">
+      <c r="B36">
         <v>2025</v>
       </c>
-      <c r="C36" s="11" t="s">
+      <c r="C36" t="s">
         <v>13</v>
       </c>
-      <c r="D36" s="12">
-        <f t="shared" si="2"/>
+      <c r="D36" s="1">
+        <f t="shared" si="4"/>
         <v>383.21504792814983</v>
       </c>
-      <c r="E36" s="11"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="11"/>
-      <c r="I36" s="11"/>
-      <c r="J36" s="11"/>
-      <c r="K36" s="11"/>
-      <c r="L36" s="11"/>
-      <c r="M36" s="11"/>
-      <c r="N36" s="11"/>
-      <c r="O36" s="11"/>
-      <c r="P36" s="11"/>
-      <c r="Q36" s="11"/>
-      <c r="R36" s="13"/>
+      <c r="R36" s="11"/>
     </row>
     <row r="37" spans="1:18">
       <c r="A37" s="10">
         <v>36</v>
       </c>
-      <c r="B37" s="11">
+      <c r="B37">
         <v>2025</v>
       </c>
-      <c r="C37" s="11" t="s">
+      <c r="C37" t="s">
         <v>14</v>
       </c>
-      <c r="D37" s="12">
-        <f t="shared" si="2"/>
+      <c r="D37" s="1">
+        <f t="shared" si="4"/>
         <v>421.53655272096483</v>
       </c>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="11"/>
-      <c r="I37" s="11"/>
-      <c r="J37" s="11"/>
-      <c r="K37" s="11"/>
-      <c r="L37" s="11"/>
-      <c r="M37" s="11"/>
-      <c r="N37" s="11"/>
-      <c r="O37" s="11"/>
-      <c r="P37" s="11"/>
-      <c r="Q37" s="11"/>
-      <c r="R37" s="13"/>
+      <c r="R37" s="11"/>
     </row>
     <row r="38" spans="1:18">
-      <c r="A38" s="19">
+      <c r="A38" s="16">
         <v>37</v>
       </c>
-      <c r="B38" s="20">
+      <c r="B38" s="17">
         <v>2026</v>
       </c>
-      <c r="C38" s="20" t="s">
+      <c r="C38" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="D38" s="21">
-        <f t="shared" si="2"/>
+      <c r="D38" s="18">
+        <f t="shared" si="4"/>
         <v>463.69020799306134</v>
       </c>
-      <c r="E38" s="20"/>
-      <c r="F38" s="20"/>
-      <c r="G38" s="20"/>
-      <c r="H38" s="20"/>
-      <c r="I38" s="20"/>
-      <c r="J38" s="20"/>
-      <c r="K38" s="20"/>
-      <c r="L38" s="20"/>
-      <c r="M38" s="20"/>
-      <c r="N38" s="20"/>
-      <c r="O38" s="20"/>
-      <c r="P38" s="20"/>
-      <c r="Q38" s="20"/>
-      <c r="R38" s="22"/>
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="17"/>
+      <c r="H38" s="17"/>
+      <c r="I38" s="17"/>
+      <c r="J38" s="17"/>
+      <c r="K38" s="17"/>
+      <c r="L38" s="17"/>
+      <c r="M38" s="17"/>
+      <c r="N38" s="17"/>
+      <c r="O38" s="17"/>
+      <c r="P38" s="17"/>
+      <c r="Q38" s="17"/>
+      <c r="R38" s="19"/>
     </row>
     <row r="39" spans="1:18">
-      <c r="A39" s="23">
+      <c r="A39" s="20">
         <v>38</v>
       </c>
-      <c r="B39" s="11">
+      <c r="B39">
         <v>2026</v>
       </c>
-      <c r="C39" s="11" t="s">
+      <c r="C39" t="s">
         <v>4</v>
       </c>
-      <c r="D39" s="12">
-        <f t="shared" si="2"/>
+      <c r="D39" s="1">
+        <f t="shared" si="4"/>
         <v>510.05922879236749</v>
       </c>
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="11"/>
-      <c r="H39" s="11"/>
-      <c r="I39" s="11"/>
-      <c r="J39" s="11"/>
-      <c r="K39" s="11"/>
-      <c r="L39" s="11"/>
-      <c r="M39" s="11"/>
-      <c r="N39" s="11"/>
-      <c r="O39" s="11"/>
-      <c r="P39" s="11"/>
-      <c r="Q39" s="11"/>
-      <c r="R39" s="24"/>
+      <c r="R39" s="21"/>
     </row>
     <row r="40" spans="1:18">
-      <c r="A40" s="23">
+      <c r="A40" s="20">
         <v>39</v>
       </c>
-      <c r="B40" s="11">
+      <c r="B40">
         <v>2026</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="C40" t="s">
         <v>5</v>
       </c>
-      <c r="D40" s="12">
-        <f t="shared" si="2"/>
+      <c r="D40" s="1">
+        <f t="shared" si="4"/>
         <v>561.06515167160433</v>
       </c>
-      <c r="E40" s="11"/>
-      <c r="F40" s="11"/>
-      <c r="G40" s="11"/>
-      <c r="H40" s="11"/>
-      <c r="I40" s="11"/>
-      <c r="J40" s="11"/>
-      <c r="K40" s="11"/>
-      <c r="L40" s="11"/>
-      <c r="M40" s="11"/>
-      <c r="N40" s="11"/>
-      <c r="O40" s="11"/>
-      <c r="P40" s="11"/>
-      <c r="Q40" s="11"/>
-      <c r="R40" s="24"/>
+      <c r="R40" s="21"/>
     </row>
     <row r="41" spans="1:18">
-      <c r="A41" s="23">
+      <c r="A41" s="20">
         <v>40</v>
       </c>
-      <c r="B41" s="11">
+      <c r="B41">
         <v>2026</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="C41" t="s">
         <v>6</v>
       </c>
-      <c r="D41" s="12">
-        <f t="shared" si="2"/>
+      <c r="D41" s="1">
+        <f t="shared" si="4"/>
         <v>617.17166683876485</v>
       </c>
-      <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="11"/>
-      <c r="I41" s="11"/>
-      <c r="J41" s="11"/>
-      <c r="K41" s="11"/>
-      <c r="L41" s="11"/>
-      <c r="M41" s="11"/>
-      <c r="N41" s="11"/>
-      <c r="O41" s="11"/>
-      <c r="P41" s="11"/>
-      <c r="Q41" s="11"/>
-      <c r="R41" s="24"/>
+      <c r="R41" s="21"/>
     </row>
     <row r="42" spans="1:18">
-      <c r="A42" s="23">
+      <c r="A42" s="20">
         <v>41</v>
       </c>
-      <c r="B42" s="11">
+      <c r="B42">
         <v>2026</v>
       </c>
-      <c r="C42" s="11" t="s">
+      <c r="C42" t="s">
         <v>7</v>
       </c>
-      <c r="D42" s="12">
-        <f t="shared" si="2"/>
+      <c r="D42" s="1">
+        <f t="shared" si="4"/>
         <v>678.88883352264133</v>
       </c>
-      <c r="E42" s="11"/>
-      <c r="F42" s="11"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="11"/>
-      <c r="I42" s="11"/>
-      <c r="J42" s="11"/>
-      <c r="K42" s="11"/>
-      <c r="L42" s="11"/>
-      <c r="M42" s="11"/>
-      <c r="N42" s="11"/>
-      <c r="O42" s="11"/>
-      <c r="P42" s="11"/>
-      <c r="Q42" s="11"/>
-      <c r="R42" s="24"/>
+      <c r="R42" s="21"/>
     </row>
     <row r="43" spans="1:18">
-      <c r="A43" s="23">
+      <c r="A43" s="20">
         <v>42</v>
       </c>
-      <c r="B43" s="11">
+      <c r="B43">
         <v>2026</v>
       </c>
-      <c r="C43" s="11" t="s">
+      <c r="C43" t="s">
         <v>8</v>
       </c>
-      <c r="D43" s="12">
-        <f t="shared" si="2"/>
+      <c r="D43" s="1">
+        <f t="shared" si="4"/>
         <v>746.77771687490554</v>
       </c>
-      <c r="E43" s="11"/>
-      <c r="F43" s="11"/>
-      <c r="G43" s="11"/>
-      <c r="H43" s="11"/>
-      <c r="I43" s="11"/>
-      <c r="J43" s="11"/>
-      <c r="K43" s="11"/>
-      <c r="L43" s="11"/>
-      <c r="M43" s="11"/>
-      <c r="N43" s="11"/>
-      <c r="O43" s="11"/>
-      <c r="P43" s="11"/>
-      <c r="Q43" s="11"/>
-      <c r="R43" s="24"/>
+      <c r="R43" s="21"/>
     </row>
     <row r="44" spans="1:18">
-      <c r="A44" s="23">
+      <c r="A44" s="20">
         <v>43</v>
       </c>
-      <c r="B44" s="11">
+      <c r="B44">
         <v>2026</v>
       </c>
-      <c r="C44" s="11" t="s">
+      <c r="C44" t="s">
         <v>9</v>
       </c>
-      <c r="D44" s="12">
-        <f t="shared" si="2"/>
+      <c r="D44" s="1">
+        <f t="shared" si="4"/>
         <v>821.45548856239611</v>
       </c>
-      <c r="E44" s="11"/>
-      <c r="F44" s="11"/>
-      <c r="G44" s="11"/>
-      <c r="H44" s="11"/>
-      <c r="I44" s="11"/>
-      <c r="J44" s="11"/>
-      <c r="K44" s="11"/>
-      <c r="L44" s="11"/>
-      <c r="M44" s="11"/>
-      <c r="N44" s="11"/>
-      <c r="O44" s="11"/>
-      <c r="P44" s="11"/>
-      <c r="Q44" s="11"/>
-      <c r="R44" s="24"/>
+      <c r="R44" s="21"/>
     </row>
     <row r="45" spans="1:18">
-      <c r="A45" s="23">
+      <c r="A45" s="20">
         <v>44</v>
       </c>
-      <c r="B45" s="11">
+      <c r="B45">
         <v>2026</v>
       </c>
-      <c r="C45" s="11" t="s">
+      <c r="C45" t="s">
         <v>10</v>
       </c>
-      <c r="D45" s="12">
-        <f t="shared" si="2"/>
+      <c r="D45" s="1">
+        <f t="shared" si="4"/>
         <v>903.60103741863577</v>
       </c>
-      <c r="E45" s="11"/>
-      <c r="F45" s="11"/>
-      <c r="G45" s="11"/>
-      <c r="H45" s="11"/>
-      <c r="I45" s="11"/>
-      <c r="J45" s="11"/>
-      <c r="K45" s="11"/>
-      <c r="L45" s="11"/>
-      <c r="M45" s="11"/>
-      <c r="N45" s="11"/>
-      <c r="O45" s="11"/>
-      <c r="P45" s="11"/>
-      <c r="Q45" s="11"/>
-      <c r="R45" s="24"/>
+      <c r="R45" s="21"/>
     </row>
     <row r="46" spans="1:18">
-      <c r="A46" s="23">
+      <c r="A46" s="20">
         <v>45</v>
       </c>
-      <c r="B46" s="11">
+      <c r="B46">
         <v>2026</v>
       </c>
-      <c r="C46" s="11" t="s">
+      <c r="C46" t="s">
         <v>11</v>
       </c>
-      <c r="D46" s="12">
-        <f t="shared" si="2"/>
+      <c r="D46" s="1">
+        <f t="shared" si="4"/>
         <v>993.96114116049944</v>
       </c>
-      <c r="E46" s="11"/>
-      <c r="F46" s="11"/>
-      <c r="G46" s="11"/>
-      <c r="H46" s="11"/>
-      <c r="I46" s="11"/>
-      <c r="J46" s="11"/>
-      <c r="K46" s="11"/>
-      <c r="L46" s="11"/>
-      <c r="M46" s="11"/>
-      <c r="N46" s="11"/>
-      <c r="O46" s="11"/>
-      <c r="P46" s="11"/>
-      <c r="Q46" s="11"/>
-      <c r="R46" s="24"/>
+      <c r="R46" s="21"/>
     </row>
     <row r="47" spans="1:18">
-      <c r="A47" s="23">
+      <c r="A47" s="20">
         <v>46</v>
       </c>
-      <c r="B47" s="11">
+      <c r="B47">
         <v>2026</v>
       </c>
-      <c r="C47" s="11" t="s">
+      <c r="C47" t="s">
         <v>12</v>
       </c>
-      <c r="D47" s="12">
-        <f t="shared" si="2"/>
+      <c r="D47" s="1">
+        <f t="shared" si="4"/>
         <v>1093.3572552765495</v>
       </c>
-      <c r="E47" s="11"/>
-      <c r="F47" s="11"/>
-      <c r="G47" s="11"/>
-      <c r="H47" s="11"/>
-      <c r="I47" s="11"/>
-      <c r="J47" s="11"/>
-      <c r="K47" s="11"/>
-      <c r="L47" s="11"/>
-      <c r="M47" s="11"/>
-      <c r="N47" s="11"/>
-      <c r="O47" s="11"/>
-      <c r="P47" s="11"/>
-      <c r="Q47" s="11"/>
-      <c r="R47" s="24"/>
+      <c r="R47" s="21"/>
     </row>
     <row r="48" spans="1:18">
-      <c r="A48" s="23">
+      <c r="A48" s="20">
         <v>47</v>
       </c>
-      <c r="B48" s="11">
+      <c r="B48">
         <v>2026</v>
       </c>
-      <c r="C48" s="11" t="s">
+      <c r="C48" t="s">
         <v>13</v>
       </c>
-      <c r="D48" s="12">
-        <f t="shared" si="2"/>
+      <c r="D48" s="1">
+        <f t="shared" si="4"/>
         <v>1202.6929808042046</v>
       </c>
-      <c r="E48" s="11"/>
-      <c r="F48" s="11"/>
-      <c r="G48" s="11"/>
-      <c r="H48" s="11"/>
-      <c r="I48" s="11"/>
-      <c r="J48" s="11"/>
-      <c r="K48" s="11"/>
-      <c r="L48" s="11"/>
-      <c r="M48" s="11"/>
-      <c r="N48" s="11"/>
-      <c r="O48" s="11"/>
-      <c r="P48" s="11"/>
-      <c r="Q48" s="11"/>
-      <c r="R48" s="24"/>
+      <c r="R48" s="21"/>
     </row>
     <row r="49" spans="1:18">
-      <c r="A49" s="25">
+      <c r="A49" s="22">
         <v>48</v>
       </c>
-      <c r="B49" s="26">
+      <c r="B49" s="23">
         <v>2026</v>
       </c>
-      <c r="C49" s="26" t="s">
+      <c r="C49" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="D49" s="27">
-        <f t="shared" si="2"/>
+      <c r="D49" s="24">
+        <f t="shared" si="4"/>
         <v>1322.9622788846252</v>
       </c>
-      <c r="E49" s="26"/>
-      <c r="F49" s="26"/>
-      <c r="G49" s="26"/>
-      <c r="H49" s="26"/>
-      <c r="I49" s="26"/>
-      <c r="J49" s="26"/>
-      <c r="K49" s="26"/>
-      <c r="L49" s="26"/>
-      <c r="M49" s="26"/>
-      <c r="N49" s="26"/>
-      <c r="O49" s="26"/>
-      <c r="P49" s="26"/>
-      <c r="Q49" s="26"/>
-      <c r="R49" s="28"/>
+      <c r="E49" s="23"/>
+      <c r="F49" s="23"/>
+      <c r="G49" s="23"/>
+      <c r="H49" s="23"/>
+      <c r="I49" s="23"/>
+      <c r="J49" s="23"/>
+      <c r="K49" s="23"/>
+      <c r="L49" s="23"/>
+      <c r="M49" s="23"/>
+      <c r="N49" s="23"/>
+      <c r="O49" s="23"/>
+      <c r="P49" s="23"/>
+      <c r="Q49" s="23"/>
+      <c r="R49" s="25"/>
     </row>
     <row r="50" spans="1:18">
-      <c r="A50" s="19">
+      <c r="A50" s="16">
         <v>49</v>
       </c>
-      <c r="B50" s="20">
+      <c r="B50" s="17">
         <v>2027</v>
       </c>
-      <c r="C50" s="20" t="s">
+      <c r="C50" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="D50" s="21">
-        <f t="shared" si="2"/>
+      <c r="D50" s="18">
+        <f t="shared" si="4"/>
         <v>1455.2585067730879</v>
       </c>
-      <c r="E50" s="20"/>
-      <c r="F50" s="20"/>
-      <c r="G50" s="20"/>
-      <c r="H50" s="20"/>
-      <c r="I50" s="20"/>
-      <c r="J50" s="20"/>
-      <c r="K50" s="20"/>
-      <c r="L50" s="20"/>
-      <c r="M50" s="20"/>
-      <c r="N50" s="20"/>
-      <c r="O50" s="20"/>
-      <c r="P50" s="20"/>
-      <c r="Q50" s="20"/>
-      <c r="R50" s="22"/>
+      <c r="E50" s="17"/>
+      <c r="F50" s="17"/>
+      <c r="G50" s="17"/>
+      <c r="H50" s="17"/>
+      <c r="I50" s="17"/>
+      <c r="J50" s="17"/>
+      <c r="K50" s="17"/>
+      <c r="L50" s="17"/>
+      <c r="M50" s="17"/>
+      <c r="N50" s="17"/>
+      <c r="O50" s="17"/>
+      <c r="P50" s="17"/>
+      <c r="Q50" s="17"/>
+      <c r="R50" s="19"/>
     </row>
     <row r="51" spans="1:18">
-      <c r="A51" s="23">
+      <c r="A51" s="20">
         <v>50</v>
       </c>
-      <c r="B51" s="11">
+      <c r="B51">
         <v>2027</v>
       </c>
-      <c r="C51" s="11" t="s">
+      <c r="C51" t="s">
         <v>4</v>
       </c>
-      <c r="D51" s="12">
-        <f t="shared" si="2"/>
+      <c r="D51" s="1">
+        <f t="shared" si="4"/>
         <v>1600.7843574503968</v>
       </c>
-      <c r="E51" s="11"/>
-      <c r="F51" s="11"/>
-      <c r="G51" s="11"/>
-      <c r="H51" s="11"/>
-      <c r="I51" s="11"/>
-      <c r="J51" s="11"/>
-      <c r="K51" s="11"/>
-      <c r="L51" s="11"/>
-      <c r="M51" s="11"/>
-      <c r="N51" s="11"/>
-      <c r="O51" s="11"/>
-      <c r="P51" s="11"/>
-      <c r="Q51" s="11"/>
-      <c r="R51" s="24"/>
+      <c r="R51" s="21"/>
     </row>
     <row r="52" spans="1:18">
-      <c r="A52" s="23">
+      <c r="A52" s="20">
         <v>51</v>
       </c>
-      <c r="B52" s="11">
+      <c r="B52">
         <v>2027</v>
       </c>
-      <c r="C52" s="11" t="s">
+      <c r="C52" t="s">
         <v>5</v>
       </c>
-      <c r="D52" s="12">
-        <f t="shared" si="2"/>
+      <c r="D52" s="1">
+        <f t="shared" si="4"/>
         <v>1760.8627931954366</v>
       </c>
-      <c r="E52" s="11"/>
-      <c r="F52" s="11"/>
-      <c r="G52" s="11"/>
-      <c r="H52" s="11"/>
-      <c r="I52" s="11"/>
-      <c r="J52" s="11"/>
-      <c r="K52" s="11"/>
-      <c r="L52" s="11"/>
-      <c r="M52" s="11"/>
-      <c r="N52" s="11"/>
-      <c r="O52" s="11"/>
-      <c r="P52" s="11"/>
-      <c r="Q52" s="11"/>
-      <c r="R52" s="24"/>
+      <c r="R52" s="21"/>
     </row>
     <row r="53" spans="1:18">
-      <c r="A53" s="23">
+      <c r="A53" s="20">
         <v>52</v>
       </c>
-      <c r="B53" s="11">
+      <c r="B53">
         <v>2027</v>
       </c>
-      <c r="C53" s="11" t="s">
+      <c r="C53" t="s">
         <v>6</v>
       </c>
-      <c r="D53" s="12">
-        <f t="shared" si="2"/>
+      <c r="D53" s="1">
+        <f t="shared" si="4"/>
         <v>1936.9490725149803</v>
       </c>
-      <c r="E53" s="11"/>
-      <c r="F53" s="11"/>
-      <c r="G53" s="11"/>
-      <c r="H53" s="11"/>
-      <c r="I53" s="11"/>
-      <c r="J53" s="11"/>
-      <c r="K53" s="11"/>
-      <c r="L53" s="11"/>
-      <c r="M53" s="11"/>
-      <c r="N53" s="11"/>
-      <c r="O53" s="11"/>
-      <c r="P53" s="11"/>
-      <c r="Q53" s="11"/>
-      <c r="R53" s="24"/>
+      <c r="R53" s="21"/>
     </row>
     <row r="54" spans="1:18">
-      <c r="A54" s="23">
+      <c r="A54" s="20">
         <v>53</v>
       </c>
-      <c r="B54" s="11">
+      <c r="B54">
         <v>2027</v>
       </c>
-      <c r="C54" s="11" t="s">
+      <c r="C54" t="s">
         <v>7</v>
       </c>
-      <c r="D54" s="12">
-        <f t="shared" si="2"/>
+      <c r="D54" s="1">
+        <f t="shared" si="4"/>
         <v>2130.6439797664784</v>
       </c>
-      <c r="E54" s="11"/>
-      <c r="F54" s="11"/>
-      <c r="G54" s="11"/>
-      <c r="H54" s="11"/>
-      <c r="I54" s="11"/>
-      <c r="J54" s="11"/>
-      <c r="K54" s="11"/>
-      <c r="L54" s="11"/>
-      <c r="M54" s="11"/>
-      <c r="N54" s="11"/>
-      <c r="O54" s="11"/>
-      <c r="P54" s="11"/>
-      <c r="Q54" s="11"/>
-      <c r="R54" s="24"/>
+      <c r="R54" s="21"/>
     </row>
     <row r="55" spans="1:18">
-      <c r="A55" s="23">
+      <c r="A55" s="20">
         <v>54</v>
       </c>
-      <c r="B55" s="11">
+      <c r="B55">
         <v>2027</v>
       </c>
-      <c r="C55" s="11" t="s">
+      <c r="C55" t="s">
         <v>8</v>
       </c>
-      <c r="D55" s="12">
-        <f t="shared" si="2"/>
+      <c r="D55" s="1">
+        <f t="shared" si="4"/>
         <v>2343.7083777431267</v>
       </c>
-      <c r="E55" s="11"/>
-      <c r="F55" s="11"/>
-      <c r="G55" s="11"/>
-      <c r="H55" s="11"/>
-      <c r="I55" s="11"/>
-      <c r="J55" s="11"/>
-      <c r="K55" s="11"/>
-      <c r="L55" s="11"/>
-      <c r="M55" s="11"/>
-      <c r="N55" s="11"/>
-      <c r="O55" s="11"/>
-      <c r="P55" s="11"/>
-      <c r="Q55" s="11"/>
-      <c r="R55" s="24"/>
+      <c r="R55" s="21"/>
     </row>
     <row r="56" spans="1:18">
-      <c r="A56" s="23">
+      <c r="A56" s="20">
         <v>55</v>
       </c>
-      <c r="B56" s="11">
+      <c r="B56">
         <v>2027</v>
       </c>
-      <c r="C56" s="11" t="s">
+      <c r="C56" t="s">
         <v>9</v>
       </c>
-      <c r="D56" s="12">
-        <f t="shared" si="2"/>
+      <c r="D56" s="1">
+        <f t="shared" si="4"/>
         <v>2578.0792155174395</v>
       </c>
-      <c r="E56" s="11"/>
-      <c r="F56" s="11"/>
-      <c r="G56" s="11"/>
-      <c r="H56" s="11"/>
-      <c r="I56" s="11"/>
-      <c r="J56" s="11"/>
-      <c r="K56" s="11"/>
-      <c r="L56" s="11"/>
-      <c r="M56" s="11"/>
-      <c r="N56" s="11"/>
-      <c r="O56" s="11"/>
-      <c r="P56" s="11"/>
-      <c r="Q56" s="11"/>
-      <c r="R56" s="24"/>
+      <c r="R56" s="21"/>
     </row>
     <row r="57" spans="1:18">
-      <c r="A57" s="23">
+      <c r="A57" s="20">
         <v>56</v>
       </c>
-      <c r="B57" s="11">
+      <c r="B57">
         <v>2027</v>
       </c>
-      <c r="C57" s="11" t="s">
+      <c r="C57" t="s">
         <v>10</v>
       </c>
-      <c r="D57" s="12">
-        <f t="shared" si="2"/>
+      <c r="D57" s="1">
+        <f t="shared" si="4"/>
         <v>2835.8871370691836</v>
       </c>
-      <c r="E57" s="11"/>
-      <c r="F57" s="11"/>
-      <c r="G57" s="11"/>
-      <c r="H57" s="11"/>
-      <c r="I57" s="11"/>
-      <c r="J57" s="11"/>
-      <c r="K57" s="11"/>
-      <c r="L57" s="11"/>
-      <c r="M57" s="11"/>
-      <c r="N57" s="11"/>
-      <c r="O57" s="11"/>
-      <c r="P57" s="11"/>
-      <c r="Q57" s="11"/>
-      <c r="R57" s="24"/>
+      <c r="R57" s="21"/>
     </row>
     <row r="58" spans="1:18">
-      <c r="A58" s="23">
+      <c r="A58" s="20">
         <v>57</v>
       </c>
-      <c r="B58" s="11">
+      <c r="B58">
         <v>2027</v>
       </c>
-      <c r="C58" s="11" t="s">
+      <c r="C58" t="s">
         <v>11</v>
       </c>
-      <c r="D58" s="12">
-        <f t="shared" si="2"/>
+      <c r="D58" s="1">
+        <f t="shared" si="4"/>
         <v>3119.4758507761021</v>
       </c>
-      <c r="E58" s="11"/>
-      <c r="F58" s="11"/>
-      <c r="G58" s="11"/>
-      <c r="H58" s="11"/>
-      <c r="I58" s="11"/>
-      <c r="J58" s="11"/>
-      <c r="K58" s="11"/>
-      <c r="L58" s="11"/>
-      <c r="M58" s="11"/>
-      <c r="N58" s="11"/>
-      <c r="O58" s="11"/>
-      <c r="P58" s="11"/>
-      <c r="Q58" s="11"/>
-      <c r="R58" s="24"/>
+      <c r="R58" s="21"/>
     </row>
     <row r="59" spans="1:18">
-      <c r="A59" s="23">
+      <c r="A59" s="20">
         <v>58</v>
       </c>
-      <c r="B59" s="11">
+      <c r="B59">
         <v>2027</v>
       </c>
-      <c r="C59" s="11" t="s">
+      <c r="C59" t="s">
         <v>12</v>
       </c>
-      <c r="D59" s="12">
-        <f t="shared" si="2"/>
+      <c r="D59" s="1">
+        <f t="shared" si="4"/>
         <v>3431.4234358537128</v>
       </c>
-      <c r="E59" s="11"/>
-      <c r="F59" s="11"/>
-      <c r="G59" s="11"/>
-      <c r="H59" s="11"/>
-      <c r="I59" s="11"/>
-      <c r="J59" s="11"/>
-      <c r="K59" s="11"/>
-      <c r="L59" s="11"/>
-      <c r="M59" s="11"/>
-      <c r="N59" s="11"/>
-      <c r="O59" s="11"/>
-      <c r="P59" s="11"/>
-      <c r="Q59" s="11"/>
-      <c r="R59" s="24"/>
+      <c r="R59" s="21"/>
     </row>
     <row r="60" spans="1:18">
-      <c r="A60" s="23">
+      <c r="A60" s="20">
         <v>59</v>
       </c>
-      <c r="B60" s="11">
+      <c r="B60">
         <v>2027</v>
       </c>
-      <c r="C60" s="11" t="s">
+      <c r="C60" t="s">
         <v>13</v>
       </c>
-      <c r="D60" s="12">
-        <f t="shared" si="2"/>
+      <c r="D60" s="1">
+        <f t="shared" si="4"/>
         <v>3774.5657794390845</v>
       </c>
-      <c r="E60" s="11"/>
-      <c r="F60" s="11"/>
-      <c r="G60" s="11"/>
-      <c r="H60" s="11"/>
-      <c r="I60" s="11"/>
-      <c r="J60" s="11"/>
-      <c r="K60" s="11"/>
-      <c r="L60" s="11"/>
-      <c r="M60" s="11"/>
-      <c r="N60" s="11"/>
-      <c r="O60" s="11"/>
-      <c r="P60" s="11"/>
-      <c r="Q60" s="11"/>
-      <c r="R60" s="24"/>
+      <c r="R60" s="21"/>
     </row>
     <row r="61" spans="1:18">
-      <c r="A61" s="25">
+      <c r="A61" s="22">
         <v>60</v>
       </c>
-      <c r="B61" s="26">
+      <c r="B61" s="23">
         <v>2027</v>
       </c>
-      <c r="C61" s="26" t="s">
+      <c r="C61" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="D61" s="27">
-        <f t="shared" si="2"/>
+      <c r="D61" s="24">
+        <f t="shared" si="4"/>
         <v>4152.0223573829935</v>
       </c>
-      <c r="E61" s="26"/>
-      <c r="F61" s="26"/>
-      <c r="G61" s="26"/>
-      <c r="H61" s="26"/>
-      <c r="I61" s="26"/>
-      <c r="J61" s="26"/>
-      <c r="K61" s="26"/>
-      <c r="L61" s="26"/>
-      <c r="M61" s="26"/>
-      <c r="N61" s="26"/>
-      <c r="O61" s="26"/>
-      <c r="P61" s="26"/>
-      <c r="Q61" s="26"/>
-      <c r="R61" s="28"/>
+      <c r="E61" s="23"/>
+      <c r="F61" s="23"/>
+      <c r="G61" s="23"/>
+      <c r="H61" s="23"/>
+      <c r="I61" s="23"/>
+      <c r="J61" s="23"/>
+      <c r="K61" s="23"/>
+      <c r="L61" s="23"/>
+      <c r="M61" s="23"/>
+      <c r="N61" s="23"/>
+      <c r="O61" s="23"/>
+      <c r="P61" s="23"/>
+      <c r="Q61" s="23"/>
+      <c r="R61" s="25"/>
     </row>
     <row r="62" spans="1:18">
       <c r="A62">
@@ -2943,7 +3761,7 @@
         <v>3</v>
       </c>
       <c r="D62" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>4567.2245931212929</v>
       </c>
     </row>
@@ -2958,7 +3776,7 @@
         <v>4</v>
       </c>
       <c r="D63" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5023.9470524334229</v>
       </c>
     </row>
@@ -2973,7 +3791,7 @@
         <v>5</v>
       </c>
       <c r="D64" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>5526.3417576767652</v>
       </c>
     </row>
@@ -2988,7 +3806,7 @@
         <v>6</v>
       </c>
       <c r="D65" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6078.9759334444425</v>
       </c>
     </row>
@@ -3003,7 +3821,7 @@
         <v>7</v>
       </c>
       <c r="D66" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>6686.8735267888869</v>
       </c>
     </row>
@@ -3018,7 +3836,7 @@
         <v>8</v>
       </c>
       <c r="D67" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>7355.5608794677764</v>
       </c>
     </row>
@@ -3033,7 +3851,7 @@
         <v>9</v>
       </c>
       <c r="D68" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>8091.1169674145549</v>
       </c>
     </row>
@@ -3048,7 +3866,7 @@
         <v>10</v>
       </c>
       <c r="D69" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>8900.2286641560113</v>
       </c>
     </row>
@@ -3063,7 +3881,7 @@
         <v>11</v>
       </c>
       <c r="D70" s="1">
-        <f t="shared" ref="D70:D97" si="4">D69*1.1</f>
+        <f t="shared" ref="D70:D97" si="8">D69*1.1</f>
         <v>9790.2515305716133</v>
       </c>
     </row>
@@ -3078,7 +3896,7 @@
         <v>12</v>
       </c>
       <c r="D71" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>10769.276683628776</v>
       </c>
     </row>
@@ -3093,7 +3911,7 @@
         <v>13</v>
       </c>
       <c r="D72" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>11846.204351991653</v>
       </c>
     </row>
@@ -3108,7 +3926,7 @@
         <v>14</v>
       </c>
       <c r="D73" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>13030.824787190819</v>
       </c>
     </row>
@@ -3123,7 +3941,7 @@
         <v>3</v>
       </c>
       <c r="D74" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>14333.907265909902</v>
       </c>
     </row>
@@ -3138,7 +3956,7 @@
         <v>4</v>
       </c>
       <c r="D75" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>15767.297992500893</v>
       </c>
     </row>
@@ -3153,7 +3971,7 @@
         <v>5</v>
       </c>
       <c r="D76" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>17344.027791750985</v>
       </c>
     </row>
@@ -3168,7 +3986,7 @@
         <v>6</v>
       </c>
       <c r="D77" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>19078.430570926084</v>
       </c>
     </row>
@@ -3183,7 +4001,7 @@
         <v>7</v>
       </c>
       <c r="D78" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>20986.273628018695</v>
       </c>
     </row>
@@ -3198,7 +4016,7 @@
         <v>8</v>
       </c>
       <c r="D79" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>23084.900990820566</v>
       </c>
     </row>
@@ -3213,7 +4031,7 @@
         <v>9</v>
       </c>
       <c r="D80" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>25393.391089902623</v>
       </c>
     </row>
@@ -3228,7 +4046,7 @@
         <v>10</v>
       </c>
       <c r="D81" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>27932.730198892888</v>
       </c>
     </row>
@@ -3243,7 +4061,7 @@
         <v>11</v>
       </c>
       <c r="D82" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>30726.003218782178</v>
       </c>
     </row>
@@ -3258,7 +4076,7 @@
         <v>12</v>
       </c>
       <c r="D83" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>33798.603540660399</v>
       </c>
     </row>
@@ -3273,7 +4091,7 @@
         <v>13</v>
       </c>
       <c r="D84" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>37178.463894726439</v>
       </c>
     </row>
@@ -3288,7 +4106,7 @@
         <v>14</v>
       </c>
       <c r="D85" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>40896.310284199084</v>
       </c>
     </row>
@@ -3303,7 +4121,7 @@
         <v>3</v>
       </c>
       <c r="D86" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>44985.941312618997</v>
       </c>
     </row>
@@ -3318,7 +4136,7 @@
         <v>4</v>
       </c>
       <c r="D87" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>49484.535443880901</v>
       </c>
     </row>
@@ -3333,7 +4151,7 @@
         <v>5</v>
       </c>
       <c r="D88" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>54432.988988268997</v>
       </c>
     </row>
@@ -3348,7 +4166,7 @@
         <v>6</v>
       </c>
       <c r="D89" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>59876.287887095903</v>
       </c>
     </row>
@@ -3363,7 +4181,7 @@
         <v>7</v>
       </c>
       <c r="D90" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>65863.916675805493</v>
       </c>
     </row>
@@ -3378,7 +4196,7 @@
         <v>8</v>
       </c>
       <c r="D91" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>72450.308343386045</v>
       </c>
     </row>
@@ -3393,7 +4211,7 @@
         <v>9</v>
       </c>
       <c r="D92" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>79695.339177724658</v>
       </c>
     </row>
@@ -3408,7 +4226,7 @@
         <v>10</v>
       </c>
       <c r="D93" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>87664.873095497125</v>
       </c>
     </row>
@@ -3423,7 +4241,7 @@
         <v>11</v>
       </c>
       <c r="D94" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>96431.360405046842</v>
       </c>
     </row>
@@ -3438,7 +4256,7 @@
         <v>12</v>
       </c>
       <c r="D95" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>106074.49644555153</v>
       </c>
     </row>
@@ -3453,7 +4271,7 @@
         <v>13</v>
       </c>
       <c r="D96" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>116681.94609010669</v>
       </c>
     </row>
@@ -3468,12 +4286,13 @@
         <v>14</v>
       </c>
       <c r="D97" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="8"/>
         <v>128350.14069911737</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3481,7 +4300,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18B478A7-EA3A-EE42-9B5F-0F93A4B2BAA6}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="156" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="156" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>

</xml_diff>